<commit_message>
update data definitions in excel file
</commit_message>
<xml_diff>
--- a/data/imports/mrss-export.xlsx
+++ b/data/imports/mrss-export.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vdouglas\Documents\MRSS Development\Applications Development\Output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24816"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22360" windowHeight="19380"/>
   </bookViews>
   <sheets>
     <sheet name="DataEntry" sheetId="1" r:id="rId1"/>
@@ -39,7 +34,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="10">Form2j!$A$1:$D$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="11">'Move or Copy'!$A$1:$T$57</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -49,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="1007">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="1005">
   <si>
     <t>Maximizing Resources for Student Success</t>
   </si>
@@ -5230,16 +5225,7 @@
     <t>2012 Annual Number of FTE Staff</t>
   </si>
   <si>
-    <t>Enter the total number of student credit hours taught by part-time faculty or adjuncts in the academic unit in the 2013 academic year. This should be the number of credit hours for a course times the number of students enrolled in the course (include students who received a grade of W). For example, a 3 credit hour course with 30 enrolled students would generate 90 student credit hours. Exclude high school students taking classes taught by high school faculty in their high schools for college credit. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
-  </si>
-  <si>
     <t>FY 2012/13 Non-labor Operating Costs</t>
-  </si>
-  <si>
-    <t>Full-time equivalent (FTE) Faculty will equal total instructor credit hours taught by all full-time credit faculty in the academic unit in the 2013 academic year divided by 15. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
-  </si>
-  <si>
-    <t>Full-time equivalent (FTE) faculty will equal total instructor credit hours taught by all part-time credit faculty or adjuncts in the academic unit in the 2013 academic year divided by 15. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
   </si>
   <si>
     <r>
@@ -5273,7 +5259,10 @@
     <t>Full-time equivalent (FTE) faculty will equal instructor credit hours taught by all full-time credit faculty in the academic unit in the 2013 academic year divided by 15. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
   </si>
   <si>
-    <t>Full-time equivalent (FTE) faculty will equal total instructor credit hours taught by all full-time credit faculty in the academic unit in the 2013 academic year divided by 15. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
+    <t>Full-time equivalent (FTE) faculty will equal instructor credit hours taught by all part-time credit faculty or adjuncts in the academic unit in the 2013 academic year divided by 15. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
+  </si>
+  <si>
+    <t>Enter the number of student credit hours taught by part-time faculty or adjuncts in the academic unit in the 2013 academic year. This should be the number of credit hours for a course times the number of students enrolled in the course (include students who received a grade of W). For example, a 3 credit hour course with 30 enrolled students would generate 90 student credit hours. Exclude high school students taking classes taught by high school faculty in their high schools for college credit. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
   </si>
 </sst>
 </file>
@@ -5288,7 +5277,7 @@
     <numFmt numFmtId="166" formatCode="0.00\%\ "/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="57">
+  <fonts count="57" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -6373,26 +6362,28 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="33" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
@@ -6408,18 +6399,16 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="15"/>
     </xf>
@@ -7104,7 +7093,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7139,7 +7128,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7348,33 +7337,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:X509"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="54.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="67.7109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="51.140625" style="42" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="42" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="4" customWidth="1"/>
-    <col min="7" max="9" width="8.85546875" style="4"/>
-    <col min="10" max="10" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="54.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="67.6640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="51.1640625" style="42" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="42" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" style="4" customWidth="1"/>
+    <col min="7" max="9" width="8.83203125" style="4"/>
+    <col min="10" max="10" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="9" customFormat="1" ht="66.599999999999994" customHeight="1">
-      <c r="A1" s="243" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="243"/>
-      <c r="C1" s="243"/>
+    <row r="1" spans="1:24" s="9" customFormat="1" ht="66.5" customHeight="1">
+      <c r="A1" s="230" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="230"/>
+      <c r="C1" s="230"/>
       <c r="D1" s="42"/>
       <c r="E1" s="42"/>
       <c r="F1" s="10"/>
@@ -7407,21 +7396,21 @@
       <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:24" s="11" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A4" s="245" t="s">
+      <c r="A4" s="234" t="s">
         <v>521</v>
       </c>
-      <c r="B4" s="246"/>
-      <c r="C4" s="246"/>
+      <c r="B4" s="235"/>
+      <c r="C4" s="235"/>
       <c r="D4" s="190"/>
       <c r="E4" s="190"/>
       <c r="F4" s="10"/>
     </row>
     <row r="6" spans="1:24" ht="48.75" customHeight="1">
-      <c r="A6" s="244" t="s">
+      <c r="A6" s="233" t="s">
         <v>522</v>
       </c>
-      <c r="B6" s="244"/>
-      <c r="C6" s="244"/>
+      <c r="B6" s="233"/>
+      <c r="C6" s="233"/>
       <c r="D6" s="191"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
@@ -7451,12 +7440,12 @@
       <c r="E7" s="190"/>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:24" s="171" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A8" s="234" t="s">
+    <row r="8" spans="1:24" s="171" customFormat="1" ht="40" customHeight="1">
+      <c r="A8" s="236" t="s">
         <v>685</v>
       </c>
-      <c r="B8" s="235"/>
-      <c r="C8" s="235"/>
+      <c r="B8" s="237"/>
+      <c r="C8" s="237"/>
       <c r="D8" s="42"/>
       <c r="E8" s="42"/>
       <c r="F8" s="18"/>
@@ -7564,11 +7553,11 @@
       <c r="X11" s="69"/>
     </row>
     <row r="12" spans="1:24" s="64" customFormat="1" ht="18" customHeight="1">
-      <c r="A12" s="232" t="s">
+      <c r="A12" s="231" t="s">
         <v>456</v>
       </c>
-      <c r="B12" s="233"/>
-      <c r="C12" s="233"/>
+      <c r="B12" s="232"/>
+      <c r="C12" s="232"/>
       <c r="D12" s="192"/>
       <c r="E12" s="192"/>
       <c r="F12" s="69"/>
@@ -7780,7 +7769,7 @@
       <c r="W23" s="63"/>
       <c r="X23" s="63"/>
     </row>
-    <row r="24" spans="1:24" ht="64.5" thickBot="1">
+    <row r="24" spans="1:24" ht="49" thickBot="1">
       <c r="A24" s="75" t="s">
         <v>994</v>
       </c>
@@ -7859,7 +7848,7 @@
       </c>
       <c r="B28" s="81"/>
       <c r="C28" s="49" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="D28" s="42" t="s">
         <v>539</v>
@@ -7870,7 +7859,7 @@
     </row>
     <row r="29" spans="1:24" ht="49.5" customHeight="1" thickBot="1">
       <c r="A29" s="78" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="B29" s="80"/>
       <c r="C29" s="48" t="s">
@@ -7891,12 +7880,12 @@
       <c r="E30" s="190"/>
       <c r="F30" s="10"/>
     </row>
-    <row r="31" spans="1:24" ht="39.950000000000003" customHeight="1">
-      <c r="A31" s="234" t="s">
+    <row r="31" spans="1:24" ht="40" customHeight="1">
+      <c r="A31" s="236" t="s">
         <v>457</v>
       </c>
-      <c r="B31" s="235"/>
-      <c r="C31" s="235"/>
+      <c r="B31" s="237"/>
+      <c r="C31" s="237"/>
       <c r="F31" s="18"/>
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
@@ -8227,11 +8216,11 @@
       <c r="E49" s="190"/>
       <c r="F49" s="10"/>
     </row>
-    <row r="50" spans="1:24" ht="39.950000000000003" customHeight="1">
-      <c r="A50" s="234" t="s">
+    <row r="50" spans="1:24" ht="40" customHeight="1">
+      <c r="A50" s="236" t="s">
         <v>470</v>
       </c>
-      <c r="B50" s="235"/>
+      <c r="B50" s="237"/>
       <c r="C50" s="59"/>
       <c r="F50" s="18"/>
       <c r="G50" s="18"/>
@@ -8338,11 +8327,11 @@
       <c r="X53" s="69"/>
     </row>
     <row r="54" spans="1:24" s="64" customFormat="1" ht="18" customHeight="1">
-      <c r="A54" s="232" t="s">
+      <c r="A54" s="231" t="s">
         <v>456</v>
       </c>
-      <c r="B54" s="233"/>
-      <c r="C54" s="233"/>
+      <c r="B54" s="232"/>
+      <c r="C54" s="232"/>
       <c r="D54" s="42"/>
       <c r="E54" s="192"/>
       <c r="F54" s="69"/>
@@ -8395,8 +8384,8 @@
       <c r="A56" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="236"/>
-      <c r="C56" s="237"/>
+      <c r="B56" s="243"/>
+      <c r="C56" s="244"/>
       <c r="F56" s="32"/>
       <c r="G56" s="32"/>
       <c r="H56" s="32"/>
@@ -9126,7 +9115,7 @@
       <c r="G107" s="14"/>
       <c r="H107" s="14"/>
     </row>
-    <row r="108" spans="1:8" ht="50.1" customHeight="1" thickBot="1">
+    <row r="108" spans="1:8" ht="50" customHeight="1" thickBot="1">
       <c r="A108" s="100" t="s">
         <v>6</v>
       </c>
@@ -9281,7 +9270,7 @@
       <c r="G118" s="14"/>
       <c r="H118" s="14"/>
     </row>
-    <row r="119" spans="1:24" ht="50.1" customHeight="1" thickBot="1">
+    <row r="119" spans="1:24" ht="50" customHeight="1" thickBot="1">
       <c r="A119" s="100" t="s">
         <v>6</v>
       </c>
@@ -9364,11 +9353,11 @@
       <c r="E124" s="190"/>
       <c r="F124" s="10"/>
     </row>
-    <row r="125" spans="1:24" s="171" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A125" s="234" t="s">
+    <row r="125" spans="1:24" s="171" customFormat="1" ht="40" customHeight="1">
+      <c r="A125" s="236" t="s">
         <v>689</v>
       </c>
-      <c r="B125" s="235"/>
+      <c r="B125" s="237"/>
       <c r="C125" s="59"/>
       <c r="D125" s="42"/>
       <c r="E125" s="42"/>
@@ -9449,11 +9438,11 @@
       <c r="X127" s="69"/>
     </row>
     <row r="128" spans="1:24" s="64" customFormat="1" ht="18" customHeight="1">
-      <c r="A128" s="232" t="s">
+      <c r="A128" s="231" t="s">
         <v>456</v>
       </c>
-      <c r="B128" s="233"/>
-      <c r="C128" s="233"/>
+      <c r="B128" s="232"/>
+      <c r="C128" s="232"/>
       <c r="D128" s="33"/>
       <c r="E128" s="192"/>
       <c r="F128" s="69"/>
@@ -9506,8 +9495,8 @@
       <c r="A130" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="B130" s="236"/>
-      <c r="C130" s="237"/>
+      <c r="B130" s="243"/>
+      <c r="C130" s="244"/>
       <c r="D130" s="33"/>
       <c r="F130" s="14"/>
       <c r="G130" s="14"/>
@@ -9592,8 +9581,8 @@
       <c r="A136" s="103" t="s">
         <v>71</v>
       </c>
-      <c r="B136" s="236"/>
-      <c r="C136" s="237"/>
+      <c r="B136" s="243"/>
+      <c r="C136" s="244"/>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
       <c r="H136" s="14"/>
@@ -9758,11 +9747,11 @@
       <c r="E147" s="190"/>
       <c r="F147" s="10"/>
     </row>
-    <row r="148" spans="1:24" s="61" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A148" s="234" t="s">
+    <row r="148" spans="1:24" s="61" customFormat="1" ht="40" customHeight="1">
+      <c r="A148" s="236" t="s">
         <v>476</v>
       </c>
-      <c r="B148" s="235"/>
+      <c r="B148" s="237"/>
       <c r="C148" s="59"/>
       <c r="D148" s="42"/>
       <c r="E148" s="42"/>
@@ -9815,11 +9804,11 @@
       <c r="X149" s="69"/>
     </row>
     <row r="150" spans="1:24" s="64" customFormat="1" ht="24" customHeight="1">
-      <c r="A150" s="232" t="s">
+      <c r="A150" s="231" t="s">
         <v>478</v>
       </c>
-      <c r="B150" s="233"/>
-      <c r="C150" s="233"/>
+      <c r="B150" s="232"/>
+      <c r="C150" s="232"/>
       <c r="D150" s="42"/>
       <c r="E150" s="192"/>
       <c r="F150" s="69"/>
@@ -9869,10 +9858,10 @@
       <c r="X151" s="97"/>
     </row>
     <row r="152" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A152" s="230" t="s">
+      <c r="A152" s="245" t="s">
         <v>479</v>
       </c>
-      <c r="B152" s="231"/>
+      <c r="B152" s="246"/>
       <c r="C152" s="107"/>
       <c r="D152" s="42"/>
       <c r="E152" s="42"/>
@@ -9956,10 +9945,10 @@
       <c r="H156" s="14"/>
     </row>
     <row r="157" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A157" s="230" t="s">
+      <c r="A157" s="245" t="s">
         <v>480</v>
       </c>
-      <c r="B157" s="231"/>
+      <c r="B157" s="246"/>
       <c r="C157" s="107"/>
       <c r="D157" s="42" t="s">
         <v>740</v>
@@ -10076,7 +10065,7 @@
       <c r="G163" s="14"/>
       <c r="H163" s="14"/>
     </row>
-    <row r="164" spans="1:24" ht="47.1" customHeight="1" thickBot="1">
+    <row r="164" spans="1:24" ht="47" customHeight="1" thickBot="1">
       <c r="A164" s="201" t="s">
         <v>93</v>
       </c>
@@ -10091,7 +10080,7 @@
       <c r="G164" s="14"/>
       <c r="H164" s="14"/>
     </row>
-    <row r="165" spans="1:24" ht="50.1" customHeight="1" thickBot="1">
+    <row r="165" spans="1:24" ht="50" customHeight="1" thickBot="1">
       <c r="A165" s="203" t="s">
         <v>107</v>
       </c>
@@ -10181,7 +10170,7 @@
       <c r="G170" s="14"/>
       <c r="H170" s="14"/>
     </row>
-    <row r="171" spans="1:24" ht="44.1" customHeight="1" thickBot="1">
+    <row r="171" spans="1:24" ht="44" customHeight="1" thickBot="1">
       <c r="A171" s="201" t="s">
         <v>105</v>
       </c>
@@ -10212,10 +10201,10 @@
       <c r="H172" s="14"/>
     </row>
     <row r="173" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A173" s="230" t="s">
+      <c r="A173" s="245" t="s">
         <v>481</v>
       </c>
-      <c r="B173" s="231"/>
+      <c r="B173" s="246"/>
       <c r="C173" s="107"/>
       <c r="D173" s="42"/>
       <c r="E173" s="42"/>
@@ -10372,10 +10361,10 @@
       <c r="H183" s="14"/>
     </row>
     <row r="184" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A184" s="230" t="s">
+      <c r="A184" s="245" t="s">
         <v>491</v>
       </c>
-      <c r="B184" s="231"/>
+      <c r="B184" s="246"/>
       <c r="C184" s="107"/>
       <c r="D184" s="42"/>
       <c r="E184" s="42"/>
@@ -10442,10 +10431,10 @@
       <c r="H187" s="14"/>
     </row>
     <row r="188" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A188" s="230" t="s">
+      <c r="A188" s="245" t="s">
         <v>492</v>
       </c>
-      <c r="B188" s="231"/>
+      <c r="B188" s="246"/>
       <c r="C188" s="107"/>
       <c r="D188" s="42"/>
       <c r="E188" s="42"/>
@@ -10536,7 +10525,7 @@
       <c r="G193" s="14"/>
       <c r="H193" s="14"/>
     </row>
-    <row r="194" spans="1:24" ht="9.9499999999999993" customHeight="1">
+    <row r="194" spans="1:24" ht="10" customHeight="1">
       <c r="A194" s="23"/>
       <c r="B194" s="54"/>
       <c r="C194" s="43"/>
@@ -10545,10 +10534,10 @@
       <c r="H194" s="14"/>
     </row>
     <row r="195" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A195" s="230" t="s">
+      <c r="A195" s="245" t="s">
         <v>115</v>
       </c>
-      <c r="B195" s="231"/>
+      <c r="B195" s="246"/>
       <c r="C195" s="107"/>
       <c r="D195" s="42"/>
       <c r="E195" s="42"/>
@@ -10686,10 +10675,10 @@
       <c r="H202" s="42"/>
     </row>
     <row r="203" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A203" s="230" t="s">
+      <c r="A203" s="245" t="s">
         <v>502</v>
       </c>
-      <c r="B203" s="231"/>
+      <c r="B203" s="246"/>
       <c r="C203" s="107"/>
       <c r="D203" s="42"/>
       <c r="E203" s="42"/>
@@ -10789,11 +10778,11 @@
       <c r="E208" s="190"/>
       <c r="F208" s="10"/>
     </row>
-    <row r="209" spans="1:24" s="61" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A209" s="234" t="s">
+    <row r="209" spans="1:24" s="61" customFormat="1" ht="40" customHeight="1">
+      <c r="A209" s="236" t="s">
         <v>503</v>
       </c>
-      <c r="B209" s="235"/>
+      <c r="B209" s="237"/>
       <c r="C209" s="59"/>
       <c r="D209" s="42"/>
       <c r="E209" s="42"/>
@@ -10879,8 +10868,8 @@
       <c r="A212" s="238" t="s">
         <v>706</v>
       </c>
-      <c r="B212" s="233"/>
-      <c r="C212" s="233"/>
+      <c r="B212" s="232"/>
+      <c r="C212" s="232"/>
       <c r="D212" s="42"/>
       <c r="E212" s="192"/>
       <c r="F212" s="69"/>
@@ -10904,10 +10893,10 @@
       <c r="X212" s="69"/>
     </row>
     <row r="213" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A213" s="230" t="s">
+      <c r="A213" s="245" t="s">
         <v>504</v>
       </c>
-      <c r="B213" s="231"/>
+      <c r="B213" s="246"/>
       <c r="C213" s="107"/>
       <c r="D213" s="42"/>
       <c r="E213" s="42"/>
@@ -10993,10 +10982,10 @@
       <c r="H217" s="14"/>
     </row>
     <row r="218" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A218" s="230" t="s">
+      <c r="A218" s="245" t="s">
         <v>504</v>
       </c>
-      <c r="B218" s="231"/>
+      <c r="B218" s="246"/>
       <c r="C218" s="107"/>
       <c r="D218" s="42"/>
       <c r="E218" s="42"/>
@@ -11081,10 +11070,10 @@
       <c r="H222" s="14"/>
     </row>
     <row r="223" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A223" s="230" t="s">
+      <c r="A223" s="245" t="s">
         <v>504</v>
       </c>
-      <c r="B223" s="231"/>
+      <c r="B223" s="246"/>
       <c r="C223" s="107"/>
       <c r="D223" s="42"/>
       <c r="E223" s="42"/>
@@ -11108,7 +11097,7 @@
       <c r="W223" s="18"/>
       <c r="X223" s="18"/>
     </row>
-    <row r="224" spans="1:24" ht="33.950000000000003" customHeight="1" thickBot="1">
+    <row r="224" spans="1:24" ht="34" customHeight="1" thickBot="1">
       <c r="A224" s="197" t="s">
         <v>713</v>
       </c>
@@ -11164,10 +11153,10 @@
       <c r="H227" s="14"/>
     </row>
     <row r="228" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A228" s="230" t="s">
+      <c r="A228" s="245" t="s">
         <v>504</v>
       </c>
-      <c r="B228" s="231"/>
+      <c r="B228" s="246"/>
       <c r="C228" s="107"/>
       <c r="D228" s="42"/>
       <c r="E228" s="42"/>
@@ -11191,7 +11180,7 @@
       <c r="W228" s="18"/>
       <c r="X228" s="18"/>
     </row>
-    <row r="229" spans="1:24" ht="33.950000000000003" customHeight="1" thickBot="1">
+    <row r="229" spans="1:24" ht="34" customHeight="1" thickBot="1">
       <c r="A229" s="197" t="s">
         <v>714</v>
       </c>
@@ -11276,7 +11265,7 @@
       <c r="W233" s="18"/>
       <c r="X233" s="18"/>
     </row>
-    <row r="234" spans="1:24" s="61" customFormat="1" ht="33.950000000000003" customHeight="1" thickBot="1">
+    <row r="234" spans="1:24" s="61" customFormat="1" ht="34" customHeight="1" thickBot="1">
       <c r="A234" s="197" t="s">
         <v>716</v>
       </c>
@@ -11473,7 +11462,7 @@
       <c r="G243" s="14"/>
       <c r="H243" s="14"/>
     </row>
-    <row r="244" spans="1:24" ht="32.1" customHeight="1" thickBot="1">
+    <row r="244" spans="1:24" ht="32" customHeight="1" thickBot="1">
       <c r="A244" s="221" t="s">
         <v>130</v>
       </c>
@@ -11580,7 +11569,7 @@
       <c r="E249" s="190"/>
       <c r="F249" s="10"/>
     </row>
-    <row r="250" spans="1:24" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="250" spans="1:24" ht="20" hidden="1" customHeight="1">
       <c r="A250" s="7" t="s">
         <v>133</v>
       </c>
@@ -11601,7 +11590,7 @@
       <c r="G250" s="14"/>
       <c r="H250" s="14"/>
     </row>
-    <row r="251" spans="1:24" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="251" spans="1:24" ht="20" hidden="1" customHeight="1">
       <c r="A251" s="7" t="s">
         <v>136</v>
       </c>
@@ -11619,7 +11608,7 @@
       <c r="G251" s="14"/>
       <c r="H251" s="14"/>
     </row>
-    <row r="252" spans="1:24" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="252" spans="1:24" ht="20" hidden="1" customHeight="1">
       <c r="A252" s="7" t="s">
         <v>137</v>
       </c>
@@ -11637,7 +11626,7 @@
       <c r="G252" s="14"/>
       <c r="H252" s="14"/>
     </row>
-    <row r="253" spans="1:24" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="253" spans="1:24" ht="20" hidden="1" customHeight="1">
       <c r="A253" s="26" t="s">
         <v>139</v>
       </c>
@@ -11655,7 +11644,7 @@
       <c r="G253" s="14"/>
       <c r="H253" s="14"/>
     </row>
-    <row r="254" spans="1:24" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="254" spans="1:24" ht="20" hidden="1" customHeight="1">
       <c r="A254" s="7" t="s">
         <v>141</v>
       </c>
@@ -11673,7 +11662,7 @@
       <c r="G254" s="14"/>
       <c r="H254" s="14"/>
     </row>
-    <row r="255" spans="1:24" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="255" spans="1:24" ht="20" hidden="1" customHeight="1">
       <c r="A255" s="7" t="s">
         <v>142</v>
       </c>
@@ -11691,7 +11680,7 @@
       <c r="G255" s="14"/>
       <c r="H255" s="14"/>
     </row>
-    <row r="256" spans="1:24" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="256" spans="1:24" ht="20" hidden="1" customHeight="1">
       <c r="A256" s="26" t="s">
         <v>144</v>
       </c>
@@ -11709,7 +11698,7 @@
       <c r="G256" s="14"/>
       <c r="H256" s="14"/>
     </row>
-    <row r="257" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="257" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A257" s="7" t="s">
         <v>146</v>
       </c>
@@ -11727,7 +11716,7 @@
       <c r="G257" s="14"/>
       <c r="H257" s="14"/>
     </row>
-    <row r="258" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="258" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A258" s="7" t="s">
         <v>148</v>
       </c>
@@ -11763,7 +11752,7 @@
       <c r="G259" s="14"/>
       <c r="H259" s="14"/>
     </row>
-    <row r="260" spans="1:8" ht="27.95" hidden="1" customHeight="1">
+    <row r="260" spans="1:8" ht="28" hidden="1" customHeight="1">
       <c r="A260" s="7" t="s">
         <v>152</v>
       </c>
@@ -11799,7 +11788,7 @@
       <c r="G261" s="14"/>
       <c r="H261" s="14"/>
     </row>
-    <row r="262" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="262" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A262" s="7" t="s">
         <v>156</v>
       </c>
@@ -11853,7 +11842,7 @@
       <c r="G264" s="14"/>
       <c r="H264" s="14"/>
     </row>
-    <row r="265" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="265" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A265" s="7" t="s">
         <v>162</v>
       </c>
@@ -11871,7 +11860,7 @@
       <c r="G265" s="14"/>
       <c r="H265" s="14"/>
     </row>
-    <row r="266" spans="1:8" ht="39.950000000000003" hidden="1" customHeight="1">
+    <row r="266" spans="1:8" ht="40" hidden="1" customHeight="1">
       <c r="A266" s="7" t="s">
         <v>164</v>
       </c>
@@ -11889,7 +11878,7 @@
       <c r="G266" s="14"/>
       <c r="H266" s="14"/>
     </row>
-    <row r="267" spans="1:8" ht="24.95" hidden="1" customHeight="1">
+    <row r="267" spans="1:8" ht="25" hidden="1" customHeight="1">
       <c r="A267" s="7" t="s">
         <v>166</v>
       </c>
@@ -11925,7 +11914,7 @@
       <c r="G268" s="14"/>
       <c r="H268" s="14"/>
     </row>
-    <row r="269" spans="1:8" ht="45.95" hidden="1" customHeight="1">
+    <row r="269" spans="1:8" ht="46" hidden="1" customHeight="1">
       <c r="A269" s="7" t="s">
         <v>170</v>
       </c>
@@ -11997,7 +11986,7 @@
       <c r="G272" s="14"/>
       <c r="H272" s="14"/>
     </row>
-    <row r="273" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="273" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A273" s="7" t="s">
         <v>177</v>
       </c>
@@ -12015,7 +12004,7 @@
       <c r="G273" s="14"/>
       <c r="H273" s="14"/>
     </row>
-    <row r="274" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="274" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A274" s="7" t="s">
         <v>179</v>
       </c>
@@ -12033,7 +12022,7 @@
       <c r="G274" s="14"/>
       <c r="H274" s="14"/>
     </row>
-    <row r="275" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="275" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A275" s="7" t="s">
         <v>180</v>
       </c>
@@ -12051,7 +12040,7 @@
       <c r="G275" s="14"/>
       <c r="H275" s="14"/>
     </row>
-    <row r="276" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="276" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A276" s="26" t="s">
         <v>182</v>
       </c>
@@ -12069,7 +12058,7 @@
       <c r="G276" s="14"/>
       <c r="H276" s="14"/>
     </row>
-    <row r="277" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="277" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A277" s="7" t="s">
         <v>184</v>
       </c>
@@ -12087,7 +12076,7 @@
       <c r="G277" s="14"/>
       <c r="H277" s="14"/>
     </row>
-    <row r="278" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="278" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A278" s="7" t="s">
         <v>185</v>
       </c>
@@ -12105,7 +12094,7 @@
       <c r="G278" s="14"/>
       <c r="H278" s="14"/>
     </row>
-    <row r="279" spans="1:8" ht="24.95" hidden="1" customHeight="1">
+    <row r="279" spans="1:8" ht="25" hidden="1" customHeight="1">
       <c r="A279" s="26" t="s">
         <v>187</v>
       </c>
@@ -12123,7 +12112,7 @@
       <c r="G279" s="14"/>
       <c r="H279" s="14"/>
     </row>
-    <row r="280" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="280" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A280" s="7" t="s">
         <v>189</v>
       </c>
@@ -12177,7 +12166,7 @@
       <c r="G282" s="14"/>
       <c r="H282" s="14"/>
     </row>
-    <row r="283" spans="1:8" ht="24.95" hidden="1" customHeight="1">
+    <row r="283" spans="1:8" ht="25" hidden="1" customHeight="1">
       <c r="A283" s="7" t="s">
         <v>192</v>
       </c>
@@ -12195,7 +12184,7 @@
       <c r="G283" s="14"/>
       <c r="H283" s="14"/>
     </row>
-    <row r="284" spans="1:8" ht="36.950000000000003" hidden="1" customHeight="1">
+    <row r="284" spans="1:8" ht="37" hidden="1" customHeight="1">
       <c r="A284" s="7" t="s">
         <v>193</v>
       </c>
@@ -12321,7 +12310,7 @@
       <c r="G290" s="14"/>
       <c r="H290" s="14"/>
     </row>
-    <row r="291" spans="1:8" ht="24.95" hidden="1" customHeight="1">
+    <row r="291" spans="1:8" ht="25" hidden="1" customHeight="1">
       <c r="A291" s="7" t="s">
         <v>200</v>
       </c>
@@ -12339,7 +12328,7 @@
       <c r="G291" s="14"/>
       <c r="H291" s="14"/>
     </row>
-    <row r="292" spans="1:8" ht="36.950000000000003" hidden="1" customHeight="1">
+    <row r="292" spans="1:8" ht="37" hidden="1" customHeight="1">
       <c r="A292" s="7" t="s">
         <v>202</v>
       </c>
@@ -12357,7 +12346,7 @@
       <c r="G292" s="14"/>
       <c r="H292" s="14"/>
     </row>
-    <row r="293" spans="1:8" ht="24.95" hidden="1" customHeight="1">
+    <row r="293" spans="1:8" ht="25" hidden="1" customHeight="1">
       <c r="A293" s="7" t="s">
         <v>203</v>
       </c>
@@ -12375,7 +12364,7 @@
       <c r="G293" s="14"/>
       <c r="H293" s="14"/>
     </row>
-    <row r="294" spans="1:8" ht="48.95" hidden="1" customHeight="1">
+    <row r="294" spans="1:8" ht="49" hidden="1" customHeight="1">
       <c r="A294" s="7" t="s">
         <v>204</v>
       </c>
@@ -12393,7 +12382,7 @@
       <c r="G294" s="14"/>
       <c r="H294" s="14"/>
     </row>
-    <row r="295" spans="1:8" ht="36.950000000000003" hidden="1" customHeight="1">
+    <row r="295" spans="1:8" ht="37" hidden="1" customHeight="1">
       <c r="A295" s="7" t="s">
         <v>205</v>
       </c>
@@ -12591,7 +12580,7 @@
       <c r="G305" s="14"/>
       <c r="H305" s="14"/>
     </row>
-    <row r="306" spans="1:8" ht="24.95" hidden="1" customHeight="1">
+    <row r="306" spans="1:8" ht="25" hidden="1" customHeight="1">
       <c r="A306" s="7" t="s">
         <v>221</v>
       </c>
@@ -12609,7 +12598,7 @@
       <c r="G306" s="14"/>
       <c r="H306" s="14"/>
     </row>
-    <row r="307" spans="1:8" ht="36.950000000000003" hidden="1" customHeight="1">
+    <row r="307" spans="1:8" ht="37" hidden="1" customHeight="1">
       <c r="A307" s="7" t="s">
         <v>223</v>
       </c>
@@ -12627,7 +12616,7 @@
       <c r="G307" s="14"/>
       <c r="H307" s="14"/>
     </row>
-    <row r="308" spans="1:8" ht="26.25" hidden="1">
+    <row r="308" spans="1:8" hidden="1">
       <c r="A308" s="7" t="s">
         <v>224</v>
       </c>
@@ -12663,7 +12652,7 @@
       <c r="G309" s="14"/>
       <c r="H309" s="14"/>
     </row>
-    <row r="310" spans="1:8" ht="59.1" hidden="1" customHeight="1">
+    <row r="310" spans="1:8" ht="59" hidden="1" customHeight="1">
       <c r="A310" s="7" t="s">
         <v>226</v>
       </c>
@@ -12681,7 +12670,7 @@
       <c r="G310" s="14"/>
       <c r="H310" s="14"/>
     </row>
-    <row r="311" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="311" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A311" s="7" t="s">
         <v>227</v>
       </c>
@@ -12699,7 +12688,7 @@
       <c r="G311" s="14"/>
       <c r="H311" s="14"/>
     </row>
-    <row r="312" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="312" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A312" s="7" t="s">
         <v>228</v>
       </c>
@@ -12717,7 +12706,7 @@
       <c r="G312" s="14"/>
       <c r="H312" s="14"/>
     </row>
-    <row r="313" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="313" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A313" s="7" t="s">
         <v>229</v>
       </c>
@@ -12735,7 +12724,7 @@
       <c r="G313" s="14"/>
       <c r="H313" s="14"/>
     </row>
-    <row r="314" spans="1:8" ht="27.95" hidden="1" customHeight="1">
+    <row r="314" spans="1:8" ht="28" hidden="1" customHeight="1">
       <c r="A314" s="7" t="s">
         <v>230</v>
       </c>
@@ -12753,7 +12742,7 @@
       <c r="G314" s="14"/>
       <c r="H314" s="14"/>
     </row>
-    <row r="315" spans="1:8" ht="36.950000000000003" hidden="1" customHeight="1">
+    <row r="315" spans="1:8" ht="37" hidden="1" customHeight="1">
       <c r="A315" s="7" t="s">
         <v>231</v>
       </c>
@@ -13023,7 +13012,7 @@
       <c r="G329" s="14"/>
       <c r="H329" s="14"/>
     </row>
-    <row r="330" spans="1:8" ht="39.950000000000003" hidden="1" customHeight="1">
+    <row r="330" spans="1:8" ht="40" hidden="1" customHeight="1">
       <c r="A330" s="7" t="s">
         <v>251</v>
       </c>
@@ -13095,7 +13084,7 @@
       <c r="G333" s="14"/>
       <c r="H333" s="14"/>
     </row>
-    <row r="334" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="334" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A334" s="7" t="s">
         <v>255</v>
       </c>
@@ -13131,7 +13120,7 @@
       <c r="G335" s="14"/>
       <c r="H335" s="14"/>
     </row>
-    <row r="336" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="336" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A336" s="7" t="s">
         <v>257</v>
       </c>
@@ -13149,7 +13138,7 @@
       <c r="G336" s="14"/>
       <c r="H336" s="14"/>
     </row>
-    <row r="337" spans="1:8" ht="27.95" hidden="1" customHeight="1">
+    <row r="337" spans="1:8" ht="28" hidden="1" customHeight="1">
       <c r="A337" s="7" t="s">
         <v>258</v>
       </c>
@@ -13167,7 +13156,7 @@
       <c r="G337" s="14"/>
       <c r="H337" s="14"/>
     </row>
-    <row r="338" spans="1:8" ht="41.1" hidden="1" customHeight="1">
+    <row r="338" spans="1:8" ht="41" hidden="1" customHeight="1">
       <c r="A338" s="7" t="s">
         <v>259</v>
       </c>
@@ -13185,7 +13174,7 @@
       <c r="G338" s="14"/>
       <c r="H338" s="14"/>
     </row>
-    <row r="339" spans="1:8" ht="24.95" hidden="1" customHeight="1">
+    <row r="339" spans="1:8" ht="25" hidden="1" customHeight="1">
       <c r="A339" s="7" t="s">
         <v>260</v>
       </c>
@@ -13221,7 +13210,7 @@
       <c r="G340" s="14"/>
       <c r="H340" s="14"/>
     </row>
-    <row r="341" spans="1:8" ht="36.950000000000003" hidden="1" customHeight="1">
+    <row r="341" spans="1:8" ht="37" hidden="1" customHeight="1">
       <c r="A341" s="47" t="s">
         <v>262</v>
       </c>
@@ -13311,7 +13300,7 @@
       <c r="G345" s="14"/>
       <c r="H345" s="14"/>
     </row>
-    <row r="346" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="346" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A346" s="23" t="s">
         <v>270</v>
       </c>
@@ -13329,7 +13318,7 @@
       <c r="G346" s="14"/>
       <c r="H346" s="14"/>
     </row>
-    <row r="347" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="347" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A347" s="23" t="s">
         <v>271</v>
       </c>
@@ -13437,7 +13426,7 @@
       <c r="G352" s="14"/>
       <c r="H352" s="14"/>
     </row>
-    <row r="353" spans="1:8" ht="36.950000000000003" hidden="1" customHeight="1">
+    <row r="353" spans="1:8" ht="37" hidden="1" customHeight="1">
       <c r="A353" s="7" t="s">
         <v>279</v>
       </c>
@@ -13509,7 +13498,7 @@
       <c r="G356" s="14"/>
       <c r="H356" s="14"/>
     </row>
-    <row r="357" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="357" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A357" s="7" t="s">
         <v>283</v>
       </c>
@@ -13527,7 +13516,7 @@
       <c r="G357" s="14"/>
       <c r="H357" s="14"/>
     </row>
-    <row r="358" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="358" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A358" s="7" t="s">
         <v>284</v>
       </c>
@@ -13545,7 +13534,7 @@
       <c r="G358" s="14"/>
       <c r="H358" s="14"/>
     </row>
-    <row r="359" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="359" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A359" s="7" t="s">
         <v>285</v>
       </c>
@@ -13581,7 +13570,7 @@
       <c r="G360" s="14"/>
       <c r="H360" s="14"/>
     </row>
-    <row r="361" spans="1:8" ht="53.1" hidden="1" customHeight="1">
+    <row r="361" spans="1:8" ht="53" hidden="1" customHeight="1">
       <c r="A361" s="7" t="s">
         <v>287</v>
       </c>
@@ -13599,7 +13588,7 @@
       <c r="G361" s="14"/>
       <c r="H361" s="14"/>
     </row>
-    <row r="362" spans="1:8" ht="27.95" hidden="1" customHeight="1">
+    <row r="362" spans="1:8" ht="28" hidden="1" customHeight="1">
       <c r="A362" s="7" t="s">
         <v>289</v>
       </c>
@@ -13617,7 +13606,7 @@
       <c r="G362" s="14"/>
       <c r="H362" s="14"/>
     </row>
-    <row r="363" spans="1:8" ht="53.1" hidden="1" customHeight="1">
+    <row r="363" spans="1:8" ht="53" hidden="1" customHeight="1">
       <c r="A363" s="7" t="s">
         <v>290</v>
       </c>
@@ -13635,7 +13624,7 @@
       <c r="G363" s="14"/>
       <c r="H363" s="14"/>
     </row>
-    <row r="364" spans="1:8" ht="53.1" hidden="1" customHeight="1">
+    <row r="364" spans="1:8" ht="53" hidden="1" customHeight="1">
       <c r="A364" s="7" t="s">
         <v>291</v>
       </c>
@@ -13653,7 +13642,7 @@
       <c r="G364" s="14"/>
       <c r="H364" s="14"/>
     </row>
-    <row r="365" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="365" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A365" s="7" t="s">
         <v>292</v>
       </c>
@@ -13671,7 +13660,7 @@
       <c r="G365" s="14"/>
       <c r="H365" s="14"/>
     </row>
-    <row r="366" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="366" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A366" s="23" t="s">
         <v>294</v>
       </c>
@@ -13689,7 +13678,7 @@
       <c r="G366" s="14"/>
       <c r="H366" s="14"/>
     </row>
-    <row r="367" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="367" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A367" s="23" t="s">
         <v>295</v>
       </c>
@@ -13725,7 +13714,7 @@
       <c r="G368" s="14"/>
       <c r="H368" s="14"/>
     </row>
-    <row r="369" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="369" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A369" s="23" t="s">
         <v>299</v>
       </c>
@@ -13743,7 +13732,7 @@
       <c r="G369" s="14"/>
       <c r="H369" s="14"/>
     </row>
-    <row r="370" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="370" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A370" s="23" t="s">
         <v>300</v>
       </c>
@@ -13761,7 +13750,7 @@
       <c r="G370" s="14"/>
       <c r="H370" s="14"/>
     </row>
-    <row r="371" spans="1:8" ht="24.95" hidden="1" customHeight="1">
+    <row r="371" spans="1:8" ht="25" hidden="1" customHeight="1">
       <c r="A371" s="26" t="s">
         <v>302</v>
       </c>
@@ -13851,7 +13840,7 @@
       <c r="G375" s="14"/>
       <c r="H375" s="14"/>
     </row>
-    <row r="376" spans="1:8" ht="50.1" hidden="1" customHeight="1">
+    <row r="376" spans="1:8" ht="50" hidden="1" customHeight="1">
       <c r="A376" s="7" t="s">
         <v>308</v>
       </c>
@@ -13869,7 +13858,7 @@
       <c r="G376" s="14"/>
       <c r="H376" s="14"/>
     </row>
-    <row r="377" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="377" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A377" s="7" t="s">
         <v>309</v>
       </c>
@@ -13923,7 +13912,7 @@
       <c r="G379" s="14"/>
       <c r="H379" s="14"/>
     </row>
-    <row r="380" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="380" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A380" s="7" t="s">
         <v>312</v>
       </c>
@@ -13941,7 +13930,7 @@
       <c r="G380" s="14"/>
       <c r="H380" s="14"/>
     </row>
-    <row r="381" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="381" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A381" s="7" t="s">
         <v>313</v>
       </c>
@@ -13959,7 +13948,7 @@
       <c r="G381" s="14"/>
       <c r="H381" s="14"/>
     </row>
-    <row r="382" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="382" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A382" s="7" t="s">
         <v>314</v>
       </c>
@@ -13995,7 +13984,7 @@
       <c r="G383" s="14"/>
       <c r="H383" s="14"/>
     </row>
-    <row r="384" spans="1:8" ht="53.1" hidden="1" customHeight="1">
+    <row r="384" spans="1:8" ht="53" hidden="1" customHeight="1">
       <c r="A384" s="7" t="s">
         <v>316</v>
       </c>
@@ -14013,7 +14002,7 @@
       <c r="G384" s="14"/>
       <c r="H384" s="14"/>
     </row>
-    <row r="385" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="385" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A385" s="7" t="s">
         <v>317</v>
       </c>
@@ -14031,7 +14020,7 @@
       <c r="G385" s="14"/>
       <c r="H385" s="14"/>
     </row>
-    <row r="386" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="386" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A386" s="7" t="s">
         <v>318</v>
       </c>
@@ -14049,7 +14038,7 @@
       <c r="G386" s="14"/>
       <c r="H386" s="14"/>
     </row>
-    <row r="387" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="387" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A387" s="7" t="s">
         <v>319</v>
       </c>
@@ -14067,7 +14056,7 @@
       <c r="G387" s="14"/>
       <c r="H387" s="14"/>
     </row>
-    <row r="388" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="388" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A388" s="7" t="s">
         <v>320</v>
       </c>
@@ -14085,7 +14074,7 @@
       <c r="G388" s="14"/>
       <c r="H388" s="14"/>
     </row>
-    <row r="389" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="389" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A389" s="23" t="s">
         <v>322</v>
       </c>
@@ -14103,7 +14092,7 @@
       <c r="G389" s="14"/>
       <c r="H389" s="14"/>
     </row>
-    <row r="390" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="390" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A390" s="23" t="s">
         <v>323</v>
       </c>
@@ -14121,7 +14110,7 @@
       <c r="G390" s="14"/>
       <c r="H390" s="14"/>
     </row>
-    <row r="391" spans="1:8" ht="24.95" hidden="1" customHeight="1">
+    <row r="391" spans="1:8" ht="25" hidden="1" customHeight="1">
       <c r="A391" s="26" t="s">
         <v>325</v>
       </c>
@@ -14139,7 +14128,7 @@
       <c r="G391" s="14"/>
       <c r="H391" s="14"/>
     </row>
-    <row r="392" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="392" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A392" s="23" t="s">
         <v>327</v>
       </c>
@@ -14157,7 +14146,7 @@
       <c r="G392" s="14"/>
       <c r="H392" s="14"/>
     </row>
-    <row r="393" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="393" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A393" s="23" t="s">
         <v>328</v>
       </c>
@@ -14283,7 +14272,7 @@
       <c r="G399" s="14"/>
       <c r="H399" s="14"/>
     </row>
-    <row r="400" spans="1:8" ht="26.25" hidden="1">
+    <row r="400" spans="1:8" hidden="1">
       <c r="A400" s="7" t="s">
         <v>337</v>
       </c>
@@ -14337,7 +14326,7 @@
       <c r="G402" s="14"/>
       <c r="H402" s="14"/>
     </row>
-    <row r="403" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="403" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A403" s="7" t="s">
         <v>340</v>
       </c>
@@ -14355,7 +14344,7 @@
       <c r="G403" s="14"/>
       <c r="H403" s="14"/>
     </row>
-    <row r="404" spans="1:8" ht="24.95" hidden="1" customHeight="1">
+    <row r="404" spans="1:8" ht="25" hidden="1" customHeight="1">
       <c r="A404" s="7" t="s">
         <v>341</v>
       </c>
@@ -14373,7 +14362,7 @@
       <c r="G404" s="14"/>
       <c r="H404" s="14"/>
     </row>
-    <row r="405" spans="1:8" ht="24.95" hidden="1" customHeight="1">
+    <row r="405" spans="1:8" ht="25" hidden="1" customHeight="1">
       <c r="A405" s="7" t="s">
         <v>342</v>
       </c>
@@ -14445,7 +14434,7 @@
       <c r="G408" s="14"/>
       <c r="H408" s="14"/>
     </row>
-    <row r="409" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="409" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A409" s="7" t="s">
         <v>346</v>
       </c>
@@ -14463,7 +14452,7 @@
       <c r="G409" s="14"/>
       <c r="H409" s="14"/>
     </row>
-    <row r="410" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="410" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A410" s="7" t="s">
         <v>347</v>
       </c>
@@ -14481,7 +14470,7 @@
       <c r="G410" s="14"/>
       <c r="H410" s="14"/>
     </row>
-    <row r="411" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="411" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A411" s="7" t="s">
         <v>348</v>
       </c>
@@ -14499,7 +14488,7 @@
       <c r="G411" s="14"/>
       <c r="H411" s="14"/>
     </row>
-    <row r="412" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="412" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A412" s="23" t="s">
         <v>350</v>
       </c>
@@ -14517,7 +14506,7 @@
       <c r="G412" s="14"/>
       <c r="H412" s="14"/>
     </row>
-    <row r="413" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="413" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A413" s="23" t="s">
         <v>351</v>
       </c>
@@ -14535,7 +14524,7 @@
       <c r="G413" s="14"/>
       <c r="H413" s="14"/>
     </row>
-    <row r="414" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="414" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A414" s="26" t="s">
         <v>353</v>
       </c>
@@ -14553,7 +14542,7 @@
       <c r="G414" s="14"/>
       <c r="H414" s="14"/>
     </row>
-    <row r="415" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="415" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A415" s="23" t="s">
         <v>355</v>
       </c>
@@ -14571,7 +14560,7 @@
       <c r="G415" s="14"/>
       <c r="H415" s="14"/>
     </row>
-    <row r="416" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="416" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A416" s="23" t="s">
         <v>356</v>
       </c>
@@ -14589,7 +14578,7 @@
       <c r="G416" s="14"/>
       <c r="H416" s="14"/>
     </row>
-    <row r="417" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="417" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A417" s="26" t="s">
         <v>358</v>
       </c>
@@ -14607,7 +14596,7 @@
       <c r="G417" s="14"/>
       <c r="H417" s="14"/>
     </row>
-    <row r="418" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="418" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A418" s="7" t="s">
         <v>360</v>
       </c>
@@ -14625,7 +14614,7 @@
       <c r="G418" s="14"/>
       <c r="H418" s="14"/>
     </row>
-    <row r="419" spans="1:8" ht="35.1" hidden="1" customHeight="1">
+    <row r="419" spans="1:8" ht="35" hidden="1" customHeight="1">
       <c r="A419" s="7" t="s">
         <v>361</v>
       </c>
@@ -14751,7 +14740,7 @@
       <c r="G425" s="14"/>
       <c r="H425" s="14"/>
     </row>
-    <row r="426" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="426" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A426" s="7" t="s">
         <v>368</v>
       </c>
@@ -14769,7 +14758,7 @@
       <c r="G426" s="14"/>
       <c r="H426" s="14"/>
     </row>
-    <row r="427" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="427" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A427" s="7" t="s">
         <v>369</v>
       </c>
@@ -14787,7 +14776,7 @@
       <c r="G427" s="14"/>
       <c r="H427" s="14"/>
     </row>
-    <row r="428" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="428" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A428" s="7" t="s">
         <v>370</v>
       </c>
@@ -14823,7 +14812,7 @@
       <c r="G429" s="14"/>
       <c r="H429" s="14"/>
     </row>
-    <row r="430" spans="1:8" ht="53.1" hidden="1" customHeight="1">
+    <row r="430" spans="1:8" ht="53" hidden="1" customHeight="1">
       <c r="A430" s="7" t="s">
         <v>372</v>
       </c>
@@ -14841,7 +14830,7 @@
       <c r="G430" s="14"/>
       <c r="H430" s="14"/>
     </row>
-    <row r="431" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="431" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A431" s="7" t="s">
         <v>373</v>
       </c>
@@ -14859,7 +14848,7 @@
       <c r="G431" s="14"/>
       <c r="H431" s="14"/>
     </row>
-    <row r="432" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="432" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A432" s="7" t="s">
         <v>374</v>
       </c>
@@ -14877,7 +14866,7 @@
       <c r="G432" s="14"/>
       <c r="H432" s="14"/>
     </row>
-    <row r="433" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="433" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A433" s="7" t="s">
         <v>375</v>
       </c>
@@ -14895,7 +14884,7 @@
       <c r="G433" s="14"/>
       <c r="H433" s="14"/>
     </row>
-    <row r="434" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="434" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A434" s="7" t="s">
         <v>376</v>
       </c>
@@ -14913,7 +14902,7 @@
       <c r="G434" s="14"/>
       <c r="H434" s="14"/>
     </row>
-    <row r="435" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="435" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A435" s="23" t="s">
         <v>378</v>
       </c>
@@ -14931,7 +14920,7 @@
       <c r="G435" s="14"/>
       <c r="H435" s="14"/>
     </row>
-    <row r="436" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="436" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A436" s="23" t="s">
         <v>379</v>
       </c>
@@ -14949,7 +14938,7 @@
       <c r="G436" s="14"/>
       <c r="H436" s="14"/>
     </row>
-    <row r="437" spans="1:8" ht="24.95" hidden="1" customHeight="1">
+    <row r="437" spans="1:8" ht="25" hidden="1" customHeight="1">
       <c r="A437" s="26" t="s">
         <v>381</v>
       </c>
@@ -14967,7 +14956,7 @@
       <c r="G437" s="14"/>
       <c r="H437" s="14"/>
     </row>
-    <row r="438" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="438" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A438" s="23" t="s">
         <v>383</v>
       </c>
@@ -14985,7 +14974,7 @@
       <c r="G438" s="14"/>
       <c r="H438" s="14"/>
     </row>
-    <row r="439" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="439" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A439" s="23" t="s">
         <v>384</v>
       </c>
@@ -15003,7 +14992,7 @@
       <c r="G439" s="14"/>
       <c r="H439" s="14"/>
     </row>
-    <row r="440" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="440" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A440" s="26" t="s">
         <v>386</v>
       </c>
@@ -15021,7 +15010,7 @@
       <c r="G440" s="14"/>
       <c r="H440" s="14"/>
     </row>
-    <row r="441" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="441" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A441" s="7" t="s">
         <v>388</v>
       </c>
@@ -15093,7 +15082,7 @@
       <c r="G444" s="14"/>
       <c r="H444" s="14"/>
     </row>
-    <row r="445" spans="1:8" ht="51.95" hidden="1" customHeight="1">
+    <row r="445" spans="1:8" ht="52" hidden="1" customHeight="1">
       <c r="A445" s="7" t="s">
         <v>393</v>
       </c>
@@ -15165,7 +15154,7 @@
       <c r="G448" s="14"/>
       <c r="H448" s="14"/>
     </row>
-    <row r="449" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="449" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A449" s="7" t="s">
         <v>398</v>
       </c>
@@ -15219,7 +15208,7 @@
       <c r="G451" s="14"/>
       <c r="H451" s="14"/>
     </row>
-    <row r="452" spans="1:8" ht="24.95" hidden="1" customHeight="1">
+    <row r="452" spans="1:8" ht="25" hidden="1" customHeight="1">
       <c r="A452" s="7" t="s">
         <v>401</v>
       </c>
@@ -15291,7 +15280,7 @@
       <c r="G455" s="14"/>
       <c r="H455" s="14"/>
     </row>
-    <row r="456" spans="1:8" ht="56.1" hidden="1" customHeight="1">
+    <row r="456" spans="1:8" ht="56" hidden="1" customHeight="1">
       <c r="A456" s="7" t="s">
         <v>405</v>
       </c>
@@ -15309,7 +15298,7 @@
       <c r="G456" s="14"/>
       <c r="H456" s="14"/>
     </row>
-    <row r="457" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="457" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A457" s="7" t="s">
         <v>406</v>
       </c>
@@ -15327,7 +15316,7 @@
       <c r="G457" s="14"/>
       <c r="H457" s="14"/>
     </row>
-    <row r="458" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="458" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A458" s="23" t="s">
         <v>408</v>
       </c>
@@ -15345,7 +15334,7 @@
       <c r="G458" s="14"/>
       <c r="H458" s="14"/>
     </row>
-    <row r="459" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="459" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A459" s="23" t="s">
         <v>409</v>
       </c>
@@ -15363,7 +15352,7 @@
       <c r="G459" s="14"/>
       <c r="H459" s="14"/>
     </row>
-    <row r="460" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="460" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A460" s="26" t="s">
         <v>411</v>
       </c>
@@ -15381,7 +15370,7 @@
       <c r="G460" s="14"/>
       <c r="H460" s="14"/>
     </row>
-    <row r="461" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="461" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A461" s="23" t="s">
         <v>413</v>
       </c>
@@ -15399,7 +15388,7 @@
       <c r="G461" s="14"/>
       <c r="H461" s="14"/>
     </row>
-    <row r="462" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="462" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A462" s="23" t="s">
         <v>414</v>
       </c>
@@ -15489,7 +15478,7 @@
       <c r="G466" s="14"/>
       <c r="H466" s="14"/>
     </row>
-    <row r="467" spans="1:8" ht="24.95" hidden="1" customHeight="1">
+    <row r="467" spans="1:8" ht="25" hidden="1" customHeight="1">
       <c r="A467" s="7" t="s">
         <v>421</v>
       </c>
@@ -15507,7 +15496,7 @@
       <c r="G467" s="14"/>
       <c r="H467" s="14"/>
     </row>
-    <row r="468" spans="1:8" ht="36.950000000000003" hidden="1" customHeight="1">
+    <row r="468" spans="1:8" ht="37" hidden="1" customHeight="1">
       <c r="A468" s="7" t="s">
         <v>422</v>
       </c>
@@ -15543,7 +15532,7 @@
       <c r="G469" s="14"/>
       <c r="H469" s="14"/>
     </row>
-    <row r="470" spans="1:8" ht="57.95" hidden="1" customHeight="1">
+    <row r="470" spans="1:8" ht="58" hidden="1" customHeight="1">
       <c r="A470" s="7" t="s">
         <v>424</v>
       </c>
@@ -15651,7 +15640,7 @@
       <c r="G475" s="14"/>
       <c r="H475" s="14"/>
     </row>
-    <row r="476" spans="1:8" ht="36.950000000000003" hidden="1" customHeight="1">
+    <row r="476" spans="1:8" ht="37" hidden="1" customHeight="1">
       <c r="A476" s="7" t="s">
         <v>430</v>
       </c>
@@ -15669,7 +15658,7 @@
       <c r="G476" s="14"/>
       <c r="H476" s="14"/>
     </row>
-    <row r="477" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="477" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A477" s="7" t="s">
         <v>431</v>
       </c>
@@ -15687,7 +15676,7 @@
       <c r="G477" s="14"/>
       <c r="H477" s="14"/>
     </row>
-    <row r="478" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="478" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A478" s="7" t="s">
         <v>432</v>
       </c>
@@ -15705,7 +15694,7 @@
       <c r="G478" s="14"/>
       <c r="H478" s="14"/>
     </row>
-    <row r="479" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1">
+    <row r="479" spans="1:8" ht="20" hidden="1" customHeight="1">
       <c r="A479" s="7" t="s">
         <v>433</v>
       </c>
@@ -15777,21 +15766,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="31">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A212:C212"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A125:B125"/>
     <mergeCell ref="A213:B213"/>
     <mergeCell ref="A218:B218"/>
     <mergeCell ref="A228:B228"/>
@@ -15808,13 +15782,28 @@
     <mergeCell ref="A188:B188"/>
     <mergeCell ref="A195:B195"/>
     <mergeCell ref="A203:B203"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A212:C212"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A8:C8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A36" location="'Move or Copy'!A1" display="Link to Move or Copy"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="61" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="61" fitToHeight="0" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C
 ©National Higher Educational Benchmarking Institute
@@ -15831,7 +15820,7 @@
     <brk id="227" max="2" man="1"/>
     <brk id="248" max="2" man="1"/>
   </rowBreaks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -15842,26 +15831,26 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
   </sheetPr>
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" style="62" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="62" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" style="62" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" style="62" customWidth="1"/>
-    <col min="6" max="6" width="78.140625" style="62" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="62"/>
+    <col min="1" max="1" width="36.83203125" style="62" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="62" customWidth="1"/>
+    <col min="4" max="4" width="63.5" style="62" customWidth="1"/>
+    <col min="5" max="5" width="3.5" style="62" customWidth="1"/>
+    <col min="6" max="6" width="78.1640625" style="62" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="11" customFormat="1" ht="66.599999999999994" customHeight="1">
+    <row r="1" spans="1:25" s="11" customFormat="1" ht="66.5" customHeight="1">
       <c r="A1" s="247" t="s">
         <v>0</v>
       </c>
@@ -15890,7 +15879,7 @@
       <c r="D3" s="253"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:25" s="11" customFormat="1" ht="18.600000000000001" customHeight="1">
+    <row r="4" spans="1:25" s="11" customFormat="1" ht="18.5" customHeight="1">
       <c r="A4" s="160" t="s">
         <v>434</v>
       </c>
@@ -16039,7 +16028,7 @@
       <c r="V9" s="128"/>
       <c r="W9" s="128"/>
     </row>
-    <row r="10" spans="1:25" ht="23.1" customHeight="1" thickBot="1">
+    <row r="10" spans="1:25" ht="23" customHeight="1" thickBot="1">
       <c r="A10" s="58"/>
       <c r="C10" s="55"/>
       <c r="D10" s="29"/>
@@ -16051,7 +16040,7 @@
       <c r="D11" s="29"/>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="12" spans="1:25" ht="20" customHeight="1" thickBot="1">
       <c r="A12" s="74" t="s">
         <v>673</v>
       </c>
@@ -16081,7 +16070,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -16096,7 +16085,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -16104,7 +16093,7 @@
       <c r="H15" s="42"/>
       <c r="I15" s="42"/>
     </row>
-    <row r="16" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="16" spans="1:25" ht="20" customHeight="1" thickBot="1">
       <c r="A16" s="74" t="s">
         <v>676</v>
       </c>
@@ -16127,14 +16116,14 @@
       <c r="H17" s="42"/>
       <c r="I17" s="42"/>
     </row>
-    <row r="18" spans="1:24" ht="56.1" customHeight="1" thickBot="1">
+    <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
         <v>995</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -16149,7 +16138,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -16224,8 +16213,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -16274,7 +16263,7 @@
       <c r="W24" s="69"/>
       <c r="X24" s="69"/>
     </row>
-    <row r="25" spans="1:24" ht="16.350000000000001" customHeight="1">
+    <row r="25" spans="1:24" ht="16.25" customHeight="1">
       <c r="A25" s="142" t="s">
         <v>453</v>
       </c>
@@ -16338,7 +16327,7 @@
       </c>
       <c r="E28" s="21"/>
     </row>
-    <row r="29" spans="1:24" ht="24.75">
+    <row r="29" spans="1:24" ht="23">
       <c r="A29" s="153" t="s">
         <v>439</v>
       </c>
@@ -16349,7 +16338,7 @@
       </c>
       <c r="E29" s="21"/>
     </row>
-    <row r="30" spans="1:24" ht="24.75">
+    <row r="30" spans="1:24">
       <c r="A30" s="153" t="s">
         <v>441</v>
       </c>
@@ -16360,7 +16349,7 @@
       </c>
       <c r="E30" s="21"/>
     </row>
-    <row r="31" spans="1:24" ht="36">
+    <row r="31" spans="1:24" ht="33">
       <c r="A31" s="153" t="s">
         <v>442</v>
       </c>
@@ -16383,7 +16372,7 @@
       </c>
       <c r="E32" s="21"/>
     </row>
-    <row r="33" spans="1:6" ht="48.75">
+    <row r="33" spans="1:6" ht="34">
       <c r="A33" s="153" t="s">
         <v>445</v>
       </c>
@@ -16394,7 +16383,7 @@
       </c>
       <c r="E33" s="21"/>
     </row>
-    <row r="34" spans="1:6" ht="48.75">
+    <row r="34" spans="1:6" ht="34">
       <c r="A34" s="153" t="s">
         <v>447</v>
       </c>
@@ -16455,12 +16444,12 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" fitToHeight="2" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="65" fitToHeight="2" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C©National Higher Educational Benchmarking Institute
 Maximizing Resources for Student Success Data Entry Form:  Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -16471,26 +16460,26 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="0" tint="-0.14999847407452621"/>
   </sheetPr>
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" style="62" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="62" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" style="62" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" style="62" customWidth="1"/>
-    <col min="6" max="6" width="78.140625" style="62" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="62"/>
+    <col min="1" max="1" width="36.83203125" style="62" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="62" customWidth="1"/>
+    <col min="4" max="4" width="63.5" style="62" customWidth="1"/>
+    <col min="5" max="5" width="3.5" style="62" customWidth="1"/>
+    <col min="6" max="6" width="78.1640625" style="62" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="11" customFormat="1" ht="66.599999999999994" customHeight="1">
+    <row r="1" spans="1:25" s="11" customFormat="1" ht="66.5" customHeight="1">
       <c r="A1" s="247" t="s">
         <v>0</v>
       </c>
@@ -16519,7 +16508,7 @@
       <c r="D3" s="253"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:25" s="11" customFormat="1" ht="18.600000000000001" customHeight="1">
+    <row r="4" spans="1:25" s="11" customFormat="1" ht="18.5" customHeight="1">
       <c r="A4" s="160" t="s">
         <v>434</v>
       </c>
@@ -16668,7 +16657,7 @@
       <c r="V9" s="128"/>
       <c r="W9" s="128"/>
     </row>
-    <row r="10" spans="1:25" ht="23.1" customHeight="1" thickBot="1">
+    <row r="10" spans="1:25" ht="23" customHeight="1" thickBot="1">
       <c r="A10" s="58"/>
       <c r="C10" s="55"/>
       <c r="D10" s="29"/>
@@ -16680,7 +16669,7 @@
       <c r="D11" s="29"/>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="12" spans="1:25" ht="20" customHeight="1" thickBot="1">
       <c r="A12" s="74" t="s">
         <v>673</v>
       </c>
@@ -16710,7 +16699,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -16725,7 +16714,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -16733,7 +16722,7 @@
       <c r="H15" s="42"/>
       <c r="I15" s="42"/>
     </row>
-    <row r="16" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="16" spans="1:25" ht="20" customHeight="1" thickBot="1">
       <c r="A16" s="74" t="s">
         <v>676</v>
       </c>
@@ -16756,14 +16745,14 @@
       <c r="H17" s="42"/>
       <c r="I17" s="42"/>
     </row>
-    <row r="18" spans="1:24" ht="56.1" customHeight="1" thickBot="1">
+    <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
         <v>452</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -16778,7 +16767,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -16853,8 +16842,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -16903,7 +16892,7 @@
       <c r="W24" s="69"/>
       <c r="X24" s="69"/>
     </row>
-    <row r="25" spans="1:24" ht="16.350000000000001" customHeight="1">
+    <row r="25" spans="1:24" ht="16.25" customHeight="1">
       <c r="A25" s="142" t="s">
         <v>453</v>
       </c>
@@ -16967,7 +16956,7 @@
       </c>
       <c r="E28" s="21"/>
     </row>
-    <row r="29" spans="1:24" ht="24.75">
+    <row r="29" spans="1:24" ht="23">
       <c r="A29" s="153" t="s">
         <v>439</v>
       </c>
@@ -16978,7 +16967,7 @@
       </c>
       <c r="E29" s="21"/>
     </row>
-    <row r="30" spans="1:24" ht="24.75">
+    <row r="30" spans="1:24">
       <c r="A30" s="153" t="s">
         <v>441</v>
       </c>
@@ -16989,7 +16978,7 @@
       </c>
       <c r="E30" s="21"/>
     </row>
-    <row r="31" spans="1:24" ht="36">
+    <row r="31" spans="1:24" ht="33">
       <c r="A31" s="153" t="s">
         <v>442</v>
       </c>
@@ -17012,7 +17001,7 @@
       </c>
       <c r="E32" s="21"/>
     </row>
-    <row r="33" spans="1:6" ht="48.75">
+    <row r="33" spans="1:6" ht="34">
       <c r="A33" s="153" t="s">
         <v>445</v>
       </c>
@@ -17023,7 +17012,7 @@
       </c>
       <c r="E33" s="21"/>
     </row>
-    <row r="34" spans="1:6" ht="48.75">
+    <row r="34" spans="1:6" ht="34">
       <c r="A34" s="153" t="s">
         <v>447</v>
       </c>
@@ -17084,12 +17073,12 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" fitToHeight="2" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="65" fitToHeight="2" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C©National Higher Educational Benchmarking Institute
 Maximizing Resources for Student Success Data Entry Form:  Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -17106,18 +17095,18 @@
       <selection activeCell="AI35" sqref="AI35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="167"/>
+    <col min="1" max="16384" width="8.83203125" style="167"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="51" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="51" orientation="portrait"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="20" max="56" man="1"/>
   </colBreaks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -17131,19 +17120,19 @@
   <dimension ref="A1:Y496"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" customWidth="1"/>
-    <col min="6" max="6" width="78.140625" customWidth="1"/>
+    <col min="1" max="1" width="36.83203125" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="63.5" customWidth="1"/>
+    <col min="5" max="5" width="3.5" customWidth="1"/>
+    <col min="6" max="6" width="78.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="9" customFormat="1" ht="66.599999999999994" customHeight="1">
+    <row r="1" spans="1:25" s="9" customFormat="1" ht="66.5" customHeight="1">
       <c r="A1" s="247" t="s">
         <v>0</v>
       </c>
@@ -17179,7 +17168,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:25" s="9" customFormat="1" ht="18.600000000000001" customHeight="1">
+    <row r="4" spans="1:25" s="9" customFormat="1" ht="18.5" customHeight="1">
       <c r="A4" s="12" t="s">
         <v>434</v>
       </c>
@@ -17218,7 +17207,7 @@
       <c r="W5" s="3"/>
     </row>
     <row r="6" spans="1:25" s="171" customFormat="1" ht="36" customHeight="1">
-      <c r="A6" s="234" t="s">
+      <c r="A6" s="236" t="s">
         <v>701</v>
       </c>
       <c r="B6" s="254"/>
@@ -17328,7 +17317,7 @@
       <c r="V9" s="128"/>
       <c r="W9" s="128"/>
     </row>
-    <row r="10" spans="1:25" ht="23.1" customHeight="1" thickBot="1">
+    <row r="10" spans="1:25" ht="23" customHeight="1" thickBot="1">
       <c r="A10" s="58"/>
       <c r="C10" s="55"/>
       <c r="D10" s="29"/>
@@ -17340,7 +17329,7 @@
       <c r="D11" s="29"/>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:25" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="12" spans="1:25" s="1" customFormat="1" ht="20" customHeight="1" thickBot="1">
       <c r="A12" s="74" t="s">
         <v>673</v>
       </c>
@@ -17372,7 +17361,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="180" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="14"/>
@@ -17387,7 +17376,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="180" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="13"/>
@@ -17395,7 +17384,7 @@
       <c r="H15" s="14"/>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="1:25" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="16" spans="1:25" s="1" customFormat="1" ht="20" customHeight="1" thickBot="1">
       <c r="A16" s="74" t="s">
         <v>676</v>
       </c>
@@ -17429,7 +17418,7 @@
       <c r="B18" s="134"/>
       <c r="C18" s="135"/>
       <c r="D18" s="180" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="14"/>
@@ -17444,7 +17433,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="66"/>
       <c r="D19" s="140" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
@@ -17518,8 +17507,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -17568,7 +17557,7 @@
       <c r="W24" s="69"/>
       <c r="X24" s="69"/>
     </row>
-    <row r="25" spans="1:24" ht="16.350000000000001" customHeight="1">
+    <row r="25" spans="1:24" ht="16.25" customHeight="1">
       <c r="A25" s="142" t="s">
         <v>453</v>
       </c>
@@ -17658,7 +17647,7 @@
       <c r="E30" s="21"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:24" ht="36">
+    <row r="31" spans="1:24" ht="33">
       <c r="A31" s="153" t="s">
         <v>442</v>
       </c>
@@ -17682,7 +17671,7 @@
       <c r="E32" s="21"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" ht="48.75">
+    <row r="33" spans="1:6" ht="34">
       <c r="A33" s="153" t="s">
         <v>445</v>
       </c>
@@ -17694,7 +17683,7 @@
       <c r="E33" s="21"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6" ht="48.75">
+    <row r="34" spans="1:6" ht="34">
       <c r="A34" s="153" t="s">
         <v>447</v>
       </c>
@@ -17724,7 +17713,7 @@
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
     </row>
-    <row r="36" spans="1:6" s="62" customFormat="1" ht="12.95" customHeight="1">
+    <row r="36" spans="1:6" s="62" customFormat="1" ht="13" customHeight="1">
       <c r="A36" s="153"/>
       <c r="B36" s="155"/>
       <c r="C36" s="155"/>
@@ -18058,12 +18047,12 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" fitToHeight="2" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="65" fitToHeight="2" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C©National Higher Educational Benchmarking Institute
 Maximizing Resources for Student Success Data Entry Form:  Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -18077,20 +18066,20 @@
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" style="62" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="62" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" style="62" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" style="62" customWidth="1"/>
-    <col min="6" max="6" width="78.140625" style="62" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="62"/>
+    <col min="1" max="1" width="36.83203125" style="62" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="62" customWidth="1"/>
+    <col min="4" max="4" width="63.5" style="62" customWidth="1"/>
+    <col min="5" max="5" width="3.5" style="62" customWidth="1"/>
+    <col min="6" max="6" width="78.1640625" style="62" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="11" customFormat="1" ht="66.599999999999994" customHeight="1">
+    <row r="1" spans="1:25" s="11" customFormat="1" ht="66.5" customHeight="1">
       <c r="A1" s="247" t="s">
         <v>0</v>
       </c>
@@ -18119,7 +18108,7 @@
       <c r="D3" s="253"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:25" s="11" customFormat="1" ht="18.600000000000001" customHeight="1">
+    <row r="4" spans="1:25" s="11" customFormat="1" ht="18.5" customHeight="1">
       <c r="A4" s="160" t="s">
         <v>434</v>
       </c>
@@ -18268,7 +18257,7 @@
       <c r="V9" s="128"/>
       <c r="W9" s="128"/>
     </row>
-    <row r="10" spans="1:25" ht="23.1" customHeight="1" thickBot="1">
+    <row r="10" spans="1:25" ht="23" customHeight="1" thickBot="1">
       <c r="A10" s="58"/>
       <c r="C10" s="55"/>
       <c r="D10" s="29"/>
@@ -18280,7 +18269,7 @@
       <c r="D11" s="29"/>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="12" spans="1:25" ht="20" customHeight="1" thickBot="1">
       <c r="A12" s="74" t="s">
         <v>673</v>
       </c>
@@ -18310,7 +18299,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="180" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -18325,7 +18314,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="180" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -18333,7 +18322,7 @@
       <c r="H15" s="42"/>
       <c r="I15" s="42"/>
     </row>
-    <row r="16" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="16" spans="1:25" ht="20" customHeight="1" thickBot="1">
       <c r="A16" s="74" t="s">
         <v>676</v>
       </c>
@@ -18356,14 +18345,14 @@
       <c r="H17" s="42"/>
       <c r="I17" s="42"/>
     </row>
-    <row r="18" spans="1:24" ht="56.1" customHeight="1" thickBot="1">
+    <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
         <v>995</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="180" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -18378,7 +18367,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -18453,8 +18442,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -18503,7 +18492,7 @@
       <c r="W24" s="69"/>
       <c r="X24" s="69"/>
     </row>
-    <row r="25" spans="1:24" ht="16.350000000000001" customHeight="1">
+    <row r="25" spans="1:24" ht="16.25" customHeight="1">
       <c r="A25" s="142" t="s">
         <v>453</v>
       </c>
@@ -18578,7 +18567,7 @@
       </c>
       <c r="E29" s="21"/>
     </row>
-    <row r="30" spans="1:24" ht="24.75">
+    <row r="30" spans="1:24">
       <c r="A30" s="153" t="s">
         <v>441</v>
       </c>
@@ -18589,7 +18578,7 @@
       </c>
       <c r="E30" s="21"/>
     </row>
-    <row r="31" spans="1:24" ht="36">
+    <row r="31" spans="1:24" ht="33">
       <c r="A31" s="153" t="s">
         <v>442</v>
       </c>
@@ -18612,7 +18601,7 @@
       </c>
       <c r="E32" s="21"/>
     </row>
-    <row r="33" spans="1:6" ht="48.75">
+    <row r="33" spans="1:6" ht="34">
       <c r="A33" s="153" t="s">
         <v>445</v>
       </c>
@@ -18623,7 +18612,7 @@
       </c>
       <c r="E33" s="21"/>
     </row>
-    <row r="34" spans="1:6" ht="48.75">
+    <row r="34" spans="1:6" ht="34">
       <c r="A34" s="153" t="s">
         <v>447</v>
       </c>
@@ -18684,12 +18673,12 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" fitToHeight="2" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="65" fitToHeight="2" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C©National Higher Educational Benchmarking Institute
 Maximizing Resources for Student Success Data Entry Form:  Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -18706,17 +18695,17 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" style="62" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="62" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" style="62" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" style="62" customWidth="1"/>
-    <col min="6" max="6" width="78.140625" style="62" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="62"/>
+    <col min="1" max="1" width="36.83203125" style="62" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="62" customWidth="1"/>
+    <col min="4" max="4" width="63.5" style="62" customWidth="1"/>
+    <col min="5" max="5" width="3.5" style="62" customWidth="1"/>
+    <col min="6" max="6" width="78.1640625" style="62" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="11" customFormat="1" ht="66.599999999999994" customHeight="1">
+    <row r="1" spans="1:25" s="11" customFormat="1" ht="66.5" customHeight="1">
       <c r="A1" s="247" t="s">
         <v>0</v>
       </c>
@@ -18745,7 +18734,7 @@
       <c r="D3" s="253"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:25" s="11" customFormat="1" ht="18.600000000000001" customHeight="1">
+    <row r="4" spans="1:25" s="11" customFormat="1" ht="18.5" customHeight="1">
       <c r="A4" s="160" t="s">
         <v>434</v>
       </c>
@@ -18894,7 +18883,7 @@
       <c r="V9" s="128"/>
       <c r="W9" s="128"/>
     </row>
-    <row r="10" spans="1:25" ht="23.1" customHeight="1" thickBot="1">
+    <row r="10" spans="1:25" ht="23" customHeight="1" thickBot="1">
       <c r="A10" s="58"/>
       <c r="C10" s="55"/>
       <c r="D10" s="29"/>
@@ -18906,7 +18895,7 @@
       <c r="D11" s="29"/>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="12" spans="1:25" ht="20" customHeight="1" thickBot="1">
       <c r="A12" s="74" t="s">
         <v>673</v>
       </c>
@@ -18936,7 +18925,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -18951,7 +18940,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -18959,7 +18948,7 @@
       <c r="H15" s="42"/>
       <c r="I15" s="42"/>
     </row>
-    <row r="16" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="16" spans="1:25" ht="20" customHeight="1" thickBot="1">
       <c r="A16" s="74" t="s">
         <v>676</v>
       </c>
@@ -18982,14 +18971,14 @@
       <c r="H17" s="42"/>
       <c r="I17" s="42"/>
     </row>
-    <row r="18" spans="1:24" ht="56.1" customHeight="1" thickBot="1">
+    <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
         <v>995</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -19004,7 +18993,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -19079,8 +19068,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -19129,7 +19118,7 @@
       <c r="W24" s="69"/>
       <c r="X24" s="69"/>
     </row>
-    <row r="25" spans="1:24" ht="16.350000000000001" customHeight="1">
+    <row r="25" spans="1:24" ht="16.25" customHeight="1">
       <c r="A25" s="142" t="s">
         <v>453</v>
       </c>
@@ -19193,7 +19182,7 @@
       </c>
       <c r="E28" s="21"/>
     </row>
-    <row r="29" spans="1:24" ht="24.75">
+    <row r="29" spans="1:24" ht="23">
       <c r="A29" s="153" t="s">
         <v>439</v>
       </c>
@@ -19204,7 +19193,7 @@
       </c>
       <c r="E29" s="21"/>
     </row>
-    <row r="30" spans="1:24" ht="24.75">
+    <row r="30" spans="1:24">
       <c r="A30" s="153" t="s">
         <v>441</v>
       </c>
@@ -19215,7 +19204,7 @@
       </c>
       <c r="E30" s="21"/>
     </row>
-    <row r="31" spans="1:24" ht="36">
+    <row r="31" spans="1:24" ht="33">
       <c r="A31" s="153" t="s">
         <v>442</v>
       </c>
@@ -19238,7 +19227,7 @@
       </c>
       <c r="E32" s="21"/>
     </row>
-    <row r="33" spans="1:6" ht="48.75">
+    <row r="33" spans="1:6" ht="34">
       <c r="A33" s="153" t="s">
         <v>445</v>
       </c>
@@ -19249,7 +19238,7 @@
       </c>
       <c r="E33" s="21"/>
     </row>
-    <row r="34" spans="1:6" ht="48.75">
+    <row r="34" spans="1:6" ht="34">
       <c r="A34" s="153" t="s">
         <v>447</v>
       </c>
@@ -19310,12 +19299,12 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" fitToHeight="2" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="65" fitToHeight="2" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C©National Higher Educational Benchmarking Institute
 Maximizing Resources for Student Success Data Entry Form:  Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -19332,17 +19321,17 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" style="62" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="62" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" style="62" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" style="62" customWidth="1"/>
-    <col min="6" max="6" width="78.140625" style="62" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="62"/>
+    <col min="1" max="1" width="36.83203125" style="62" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="62" customWidth="1"/>
+    <col min="4" max="4" width="63.5" style="62" customWidth="1"/>
+    <col min="5" max="5" width="3.5" style="62" customWidth="1"/>
+    <col min="6" max="6" width="78.1640625" style="62" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="11" customFormat="1" ht="66.599999999999994" customHeight="1">
+    <row r="1" spans="1:25" s="11" customFormat="1" ht="66.5" customHeight="1">
       <c r="A1" s="247" t="s">
         <v>0</v>
       </c>
@@ -19371,7 +19360,7 @@
       <c r="D3" s="253"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:25" s="11" customFormat="1" ht="18.600000000000001" customHeight="1">
+    <row r="4" spans="1:25" s="11" customFormat="1" ht="18.5" customHeight="1">
       <c r="A4" s="160" t="s">
         <v>434</v>
       </c>
@@ -19520,7 +19509,7 @@
       <c r="V9" s="128"/>
       <c r="W9" s="128"/>
     </row>
-    <row r="10" spans="1:25" ht="23.1" customHeight="1" thickBot="1">
+    <row r="10" spans="1:25" ht="23" customHeight="1" thickBot="1">
       <c r="A10" s="58"/>
       <c r="C10" s="55"/>
       <c r="D10" s="29"/>
@@ -19532,7 +19521,7 @@
       <c r="D11" s="29"/>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="12" spans="1:25" ht="20" customHeight="1" thickBot="1">
       <c r="A12" s="74" t="s">
         <v>673</v>
       </c>
@@ -19562,7 +19551,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -19577,7 +19566,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42" t="s">
@@ -19587,7 +19576,7 @@
       <c r="H15" s="42"/>
       <c r="I15" s="42"/>
     </row>
-    <row r="16" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="16" spans="1:25" ht="20" customHeight="1" thickBot="1">
       <c r="A16" s="74" t="s">
         <v>676</v>
       </c>
@@ -19610,14 +19599,14 @@
       <c r="H17" s="42"/>
       <c r="I17" s="42"/>
     </row>
-    <row r="18" spans="1:24" ht="56.1" customHeight="1" thickBot="1">
+    <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
         <v>995</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -19632,7 +19621,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -19707,8 +19696,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -19757,7 +19746,7 @@
       <c r="W24" s="69"/>
       <c r="X24" s="69"/>
     </row>
-    <row r="25" spans="1:24" ht="16.350000000000001" customHeight="1">
+    <row r="25" spans="1:24" ht="16.25" customHeight="1">
       <c r="A25" s="142" t="s">
         <v>453</v>
       </c>
@@ -19821,7 +19810,7 @@
       </c>
       <c r="E28" s="21"/>
     </row>
-    <row r="29" spans="1:24" ht="24.75">
+    <row r="29" spans="1:24" ht="23">
       <c r="A29" s="153" t="s">
         <v>439</v>
       </c>
@@ -19832,7 +19821,7 @@
       </c>
       <c r="E29" s="21"/>
     </row>
-    <row r="30" spans="1:24" ht="24.75">
+    <row r="30" spans="1:24">
       <c r="A30" s="153" t="s">
         <v>441</v>
       </c>
@@ -19843,7 +19832,7 @@
       </c>
       <c r="E30" s="21"/>
     </row>
-    <row r="31" spans="1:24" ht="36">
+    <row r="31" spans="1:24" ht="33">
       <c r="A31" s="153" t="s">
         <v>442</v>
       </c>
@@ -19866,7 +19855,7 @@
       </c>
       <c r="E32" s="21"/>
     </row>
-    <row r="33" spans="1:6" ht="48.75">
+    <row r="33" spans="1:6" ht="34">
       <c r="A33" s="153" t="s">
         <v>445</v>
       </c>
@@ -19877,7 +19866,7 @@
       </c>
       <c r="E33" s="21"/>
     </row>
-    <row r="34" spans="1:6" ht="48.75">
+    <row r="34" spans="1:6" ht="34">
       <c r="A34" s="153" t="s">
         <v>447</v>
       </c>
@@ -19938,12 +19927,12 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" fitToHeight="2" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="65" fitToHeight="2" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C©National Higher Educational Benchmarking Institute
 Maximizing Resources for Student Success Data Entry Form:  Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -19954,26 +19943,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
   </sheetPr>
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" style="62" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="62" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" style="62" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" style="62" customWidth="1"/>
-    <col min="6" max="6" width="78.140625" style="62" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="62"/>
+    <col min="1" max="1" width="36.83203125" style="62" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="62" customWidth="1"/>
+    <col min="4" max="4" width="63.5" style="62" customWidth="1"/>
+    <col min="5" max="5" width="3.5" style="62" customWidth="1"/>
+    <col min="6" max="6" width="78.1640625" style="62" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="11" customFormat="1" ht="66.599999999999994" customHeight="1">
+    <row r="1" spans="1:25" s="11" customFormat="1" ht="66.5" customHeight="1">
       <c r="A1" s="247" t="s">
         <v>0</v>
       </c>
@@ -20002,7 +19991,7 @@
       <c r="D3" s="253"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:25" s="11" customFormat="1" ht="18.600000000000001" customHeight="1">
+    <row r="4" spans="1:25" s="11" customFormat="1" ht="18.5" customHeight="1">
       <c r="A4" s="160" t="s">
         <v>434</v>
       </c>
@@ -20151,7 +20140,7 @@
       <c r="V9" s="128"/>
       <c r="W9" s="128"/>
     </row>
-    <row r="10" spans="1:25" ht="23.1" customHeight="1" thickBot="1">
+    <row r="10" spans="1:25" ht="23" customHeight="1" thickBot="1">
       <c r="A10" s="58"/>
       <c r="C10" s="55"/>
       <c r="D10" s="29"/>
@@ -20165,7 +20154,7 @@
       <c r="D11" s="29"/>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="12" spans="1:25" ht="20" customHeight="1" thickBot="1">
       <c r="A12" s="74" t="s">
         <v>673</v>
       </c>
@@ -20195,7 +20184,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -20210,7 +20199,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -20218,7 +20207,7 @@
       <c r="H15" s="42"/>
       <c r="I15" s="42"/>
     </row>
-    <row r="16" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="16" spans="1:25" ht="20" customHeight="1" thickBot="1">
       <c r="A16" s="74" t="s">
         <v>676</v>
       </c>
@@ -20241,14 +20230,14 @@
       <c r="H17" s="42"/>
       <c r="I17" s="42"/>
     </row>
-    <row r="18" spans="1:24" ht="56.1" customHeight="1" thickBot="1">
+    <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
         <v>995</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -20263,7 +20252,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -20338,8 +20327,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -20388,7 +20377,7 @@
       <c r="W24" s="69"/>
       <c r="X24" s="69"/>
     </row>
-    <row r="25" spans="1:24" ht="16.350000000000001" customHeight="1">
+    <row r="25" spans="1:24" ht="16.25" customHeight="1">
       <c r="A25" s="142" t="s">
         <v>453</v>
       </c>
@@ -20452,7 +20441,7 @@
       </c>
       <c r="E28" s="21"/>
     </row>
-    <row r="29" spans="1:24" ht="24.75">
+    <row r="29" spans="1:24" ht="23">
       <c r="A29" s="153" t="s">
         <v>439</v>
       </c>
@@ -20463,7 +20452,7 @@
       </c>
       <c r="E29" s="21"/>
     </row>
-    <row r="30" spans="1:24" ht="24.75">
+    <row r="30" spans="1:24">
       <c r="A30" s="153" t="s">
         <v>441</v>
       </c>
@@ -20474,7 +20463,7 @@
       </c>
       <c r="E30" s="21"/>
     </row>
-    <row r="31" spans="1:24" ht="36">
+    <row r="31" spans="1:24" ht="33">
       <c r="A31" s="153" t="s">
         <v>442</v>
       </c>
@@ -20497,7 +20486,7 @@
       </c>
       <c r="E32" s="21"/>
     </row>
-    <row r="33" spans="1:6" ht="48.75">
+    <row r="33" spans="1:6" ht="34">
       <c r="A33" s="153" t="s">
         <v>445</v>
       </c>
@@ -20508,7 +20497,7 @@
       </c>
       <c r="E33" s="21"/>
     </row>
-    <row r="34" spans="1:6" ht="48.75">
+    <row r="34" spans="1:6" ht="34">
       <c r="A34" s="153" t="s">
         <v>447</v>
       </c>
@@ -20569,12 +20558,12 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" fitToHeight="2" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="65" fitToHeight="2" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C©National Higher Educational Benchmarking Institute
 Maximizing Resources for Student Success Data Entry Form:  Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -20585,26 +20574,26 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
   </sheetPr>
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" style="62" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="62" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" style="62" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" style="62" customWidth="1"/>
-    <col min="6" max="6" width="78.140625" style="62" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="62"/>
+    <col min="1" max="1" width="36.83203125" style="62" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="62" customWidth="1"/>
+    <col min="4" max="4" width="63.5" style="62" customWidth="1"/>
+    <col min="5" max="5" width="3.5" style="62" customWidth="1"/>
+    <col min="6" max="6" width="78.1640625" style="62" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="11" customFormat="1" ht="66.599999999999994" customHeight="1">
+    <row r="1" spans="1:25" s="11" customFormat="1" ht="66.5" customHeight="1">
       <c r="A1" s="247" t="s">
         <v>0</v>
       </c>
@@ -20633,7 +20622,7 @@
       <c r="D3" s="253"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:25" s="11" customFormat="1" ht="18.600000000000001" customHeight="1">
+    <row r="4" spans="1:25" s="11" customFormat="1" ht="18.5" customHeight="1">
       <c r="A4" s="160" t="s">
         <v>434</v>
       </c>
@@ -20782,7 +20771,7 @@
       <c r="V9" s="128"/>
       <c r="W9" s="128"/>
     </row>
-    <row r="10" spans="1:25" ht="23.1" customHeight="1" thickBot="1">
+    <row r="10" spans="1:25" ht="23" customHeight="1" thickBot="1">
       <c r="A10" s="58"/>
       <c r="C10" s="55"/>
       <c r="D10" s="29"/>
@@ -20794,7 +20783,7 @@
       <c r="D11" s="29"/>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="12" spans="1:25" ht="20" customHeight="1" thickBot="1">
       <c r="A12" s="74" t="s">
         <v>673</v>
       </c>
@@ -20824,7 +20813,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -20839,7 +20828,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -20847,7 +20836,7 @@
       <c r="H15" s="42"/>
       <c r="I15" s="42"/>
     </row>
-    <row r="16" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="16" spans="1:25" ht="20" customHeight="1" thickBot="1">
       <c r="A16" s="74" t="s">
         <v>676</v>
       </c>
@@ -20870,14 +20859,14 @@
       <c r="H17" s="42"/>
       <c r="I17" s="42"/>
     </row>
-    <row r="18" spans="1:24" ht="56.1" customHeight="1" thickBot="1">
+    <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
         <v>995</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -20892,7 +20881,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -20967,8 +20956,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -21017,7 +21006,7 @@
       <c r="W24" s="69"/>
       <c r="X24" s="69"/>
     </row>
-    <row r="25" spans="1:24" ht="16.350000000000001" customHeight="1">
+    <row r="25" spans="1:24" ht="16.25" customHeight="1">
       <c r="A25" s="142" t="s">
         <v>453</v>
       </c>
@@ -21081,7 +21070,7 @@
       </c>
       <c r="E28" s="21"/>
     </row>
-    <row r="29" spans="1:24" ht="24.75">
+    <row r="29" spans="1:24" ht="23">
       <c r="A29" s="153" t="s">
         <v>439</v>
       </c>
@@ -21092,7 +21081,7 @@
       </c>
       <c r="E29" s="21"/>
     </row>
-    <row r="30" spans="1:24" ht="24.75">
+    <row r="30" spans="1:24">
       <c r="A30" s="153" t="s">
         <v>441</v>
       </c>
@@ -21103,7 +21092,7 @@
       </c>
       <c r="E30" s="21"/>
     </row>
-    <row r="31" spans="1:24" ht="36">
+    <row r="31" spans="1:24" ht="33">
       <c r="A31" s="153" t="s">
         <v>442</v>
       </c>
@@ -21126,7 +21115,7 @@
       </c>
       <c r="E32" s="21"/>
     </row>
-    <row r="33" spans="1:6" ht="48.75">
+    <row r="33" spans="1:6" ht="34">
       <c r="A33" s="153" t="s">
         <v>445</v>
       </c>
@@ -21137,7 +21126,7 @@
       </c>
       <c r="E33" s="21"/>
     </row>
-    <row r="34" spans="1:6" ht="48.75">
+    <row r="34" spans="1:6" ht="34">
       <c r="A34" s="153" t="s">
         <v>447</v>
       </c>
@@ -21198,12 +21187,12 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" fitToHeight="2" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="65" fitToHeight="2" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C©National Higher Educational Benchmarking Institute
 Maximizing Resources for Student Success Data Entry Form:  Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -21214,26 +21203,26 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
   </sheetPr>
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" style="62" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="62" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" style="62" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" style="62" customWidth="1"/>
-    <col min="6" max="6" width="78.140625" style="62" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="62"/>
+    <col min="1" max="1" width="36.83203125" style="62" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="62" customWidth="1"/>
+    <col min="4" max="4" width="63.5" style="62" customWidth="1"/>
+    <col min="5" max="5" width="3.5" style="62" customWidth="1"/>
+    <col min="6" max="6" width="78.1640625" style="62" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="11" customFormat="1" ht="66.599999999999994" customHeight="1">
+    <row r="1" spans="1:25" s="11" customFormat="1" ht="66.5" customHeight="1">
       <c r="A1" s="247" t="s">
         <v>0</v>
       </c>
@@ -21262,7 +21251,7 @@
       <c r="D3" s="253"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:25" s="11" customFormat="1" ht="18.600000000000001" customHeight="1">
+    <row r="4" spans="1:25" s="11" customFormat="1" ht="18.5" customHeight="1">
       <c r="A4" s="160" t="s">
         <v>434</v>
       </c>
@@ -21411,7 +21400,7 @@
       <c r="V9" s="128"/>
       <c r="W9" s="128"/>
     </row>
-    <row r="10" spans="1:25" ht="23.1" customHeight="1" thickBot="1">
+    <row r="10" spans="1:25" ht="23" customHeight="1" thickBot="1">
       <c r="A10" s="58"/>
       <c r="C10" s="55"/>
       <c r="D10" s="29"/>
@@ -21423,7 +21412,7 @@
       <c r="D11" s="29"/>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="12" spans="1:25" ht="20" customHeight="1" thickBot="1">
       <c r="A12" s="74" t="s">
         <v>673</v>
       </c>
@@ -21453,7 +21442,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -21468,7 +21457,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -21476,7 +21465,7 @@
       <c r="H15" s="42"/>
       <c r="I15" s="42"/>
     </row>
-    <row r="16" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="16" spans="1:25" ht="20" customHeight="1" thickBot="1">
       <c r="A16" s="74" t="s">
         <v>676</v>
       </c>
@@ -21499,14 +21488,14 @@
       <c r="H17" s="42"/>
       <c r="I17" s="42"/>
     </row>
-    <row r="18" spans="1:24" ht="56.1" customHeight="1" thickBot="1">
+    <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
         <v>995</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -21521,7 +21510,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -21596,8 +21585,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -21646,7 +21635,7 @@
       <c r="W24" s="69"/>
       <c r="X24" s="69"/>
     </row>
-    <row r="25" spans="1:24" ht="16.350000000000001" customHeight="1">
+    <row r="25" spans="1:24" ht="16.25" customHeight="1">
       <c r="A25" s="142" t="s">
         <v>453</v>
       </c>
@@ -21710,7 +21699,7 @@
       </c>
       <c r="E28" s="21"/>
     </row>
-    <row r="29" spans="1:24" ht="24.75">
+    <row r="29" spans="1:24" ht="23">
       <c r="A29" s="153" t="s">
         <v>439</v>
       </c>
@@ -21721,7 +21710,7 @@
       </c>
       <c r="E29" s="21"/>
     </row>
-    <row r="30" spans="1:24" ht="24.75">
+    <row r="30" spans="1:24">
       <c r="A30" s="153" t="s">
         <v>441</v>
       </c>
@@ -21732,7 +21721,7 @@
       </c>
       <c r="E30" s="21"/>
     </row>
-    <row r="31" spans="1:24" ht="36">
+    <row r="31" spans="1:24" ht="33">
       <c r="A31" s="153" t="s">
         <v>442</v>
       </c>
@@ -21755,7 +21744,7 @@
       </c>
       <c r="E32" s="21"/>
     </row>
-    <row r="33" spans="1:6" ht="48.75">
+    <row r="33" spans="1:6" ht="34">
       <c r="A33" s="153" t="s">
         <v>445</v>
       </c>
@@ -21766,7 +21755,7 @@
       </c>
       <c r="E33" s="21"/>
     </row>
-    <row r="34" spans="1:6" ht="48.75">
+    <row r="34" spans="1:6" ht="34">
       <c r="A34" s="153" t="s">
         <v>447</v>
       </c>
@@ -21827,12 +21816,12 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" fitToHeight="2" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="65" fitToHeight="2" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C©National Higher Educational Benchmarking Institute
 Maximizing Resources for Student Success Data Entry Form:  Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -21843,26 +21832,26 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
   </sheetPr>
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" style="62" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="62" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" style="62" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" style="62" customWidth="1"/>
-    <col min="6" max="6" width="78.140625" style="62" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="62"/>
+    <col min="1" max="1" width="36.83203125" style="62" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="62" customWidth="1"/>
+    <col min="4" max="4" width="63.5" style="62" customWidth="1"/>
+    <col min="5" max="5" width="3.5" style="62" customWidth="1"/>
+    <col min="6" max="6" width="78.1640625" style="62" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="11" customFormat="1" ht="66.599999999999994" customHeight="1">
+    <row r="1" spans="1:25" s="11" customFormat="1" ht="66.5" customHeight="1">
       <c r="A1" s="247" t="s">
         <v>0</v>
       </c>
@@ -21891,7 +21880,7 @@
       <c r="D3" s="253"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:25" s="11" customFormat="1" ht="18.600000000000001" customHeight="1">
+    <row r="4" spans="1:25" s="11" customFormat="1" ht="18.5" customHeight="1">
       <c r="A4" s="160" t="s">
         <v>434</v>
       </c>
@@ -22040,7 +22029,7 @@
       <c r="V9" s="128"/>
       <c r="W9" s="128"/>
     </row>
-    <row r="10" spans="1:25" ht="23.1" customHeight="1" thickBot="1">
+    <row r="10" spans="1:25" ht="23" customHeight="1" thickBot="1">
       <c r="A10" s="58"/>
       <c r="C10" s="55"/>
       <c r="D10" s="29"/>
@@ -22052,7 +22041,7 @@
       <c r="D11" s="29"/>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="12" spans="1:25" ht="20" customHeight="1" thickBot="1">
       <c r="A12" s="74" t="s">
         <v>673</v>
       </c>
@@ -22082,7 +22071,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -22097,7 +22086,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -22105,7 +22094,7 @@
       <c r="H15" s="42"/>
       <c r="I15" s="42"/>
     </row>
-    <row r="16" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="16" spans="1:25" ht="20" customHeight="1" thickBot="1">
       <c r="A16" s="74" t="s">
         <v>676</v>
       </c>
@@ -22128,14 +22117,14 @@
       <c r="H17" s="42"/>
       <c r="I17" s="42"/>
     </row>
-    <row r="18" spans="1:24" ht="56.1" customHeight="1" thickBot="1">
+    <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
         <v>995</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -22150,7 +22139,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>998</v>
+        <v>1004</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -22225,8 +22214,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -22275,7 +22264,7 @@
       <c r="W24" s="69"/>
       <c r="X24" s="69"/>
     </row>
-    <row r="25" spans="1:24" ht="16.350000000000001" customHeight="1">
+    <row r="25" spans="1:24" ht="16.25" customHeight="1">
       <c r="A25" s="142" t="s">
         <v>453</v>
       </c>
@@ -22339,7 +22328,7 @@
       </c>
       <c r="E28" s="21"/>
     </row>
-    <row r="29" spans="1:24" ht="24.75">
+    <row r="29" spans="1:24" ht="23">
       <c r="A29" s="153" t="s">
         <v>439</v>
       </c>
@@ -22350,7 +22339,7 @@
       </c>
       <c r="E29" s="21"/>
     </row>
-    <row r="30" spans="1:24" ht="24.75">
+    <row r="30" spans="1:24">
       <c r="A30" s="153" t="s">
         <v>441</v>
       </c>
@@ -22361,7 +22350,7 @@
       </c>
       <c r="E30" s="21"/>
     </row>
-    <row r="31" spans="1:24" ht="36">
+    <row r="31" spans="1:24" ht="33">
       <c r="A31" s="153" t="s">
         <v>442</v>
       </c>
@@ -22384,7 +22373,7 @@
       </c>
       <c r="E32" s="21"/>
     </row>
-    <row r="33" spans="1:6" ht="48.75">
+    <row r="33" spans="1:6" ht="34">
       <c r="A33" s="153" t="s">
         <v>445</v>
       </c>
@@ -22395,7 +22384,7 @@
       </c>
       <c r="E33" s="21"/>
     </row>
-    <row r="34" spans="1:6" ht="48.75">
+    <row r="34" spans="1:6" ht="34">
       <c r="A34" s="153" t="s">
         <v>447</v>
       </c>
@@ -22456,12 +22445,12 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" fitToHeight="2" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="65" fitToHeight="2" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C©National Higher Educational Benchmarking Institute
 Maximizing Resources for Student Success Data Entry Form:  Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
updating excel file with data definition change
</commit_message>
<xml_diff>
--- a/data/imports/mrss-export.xlsx
+++ b/data/imports/mrss-export.xlsx
@@ -5173,9 +5173,6 @@
     <t>Enter the number of student credit hours taught by part-time faculty or adjuncts in the 2013 academic year. This should be the number of credit hours for a course times the number of students enrolled in the course (include students who received a grade of W). For example, a 3 credit hour course with 30 enrolled students would generate 90 student credit hours. Exclude high school students taking classes taught by high school faculty in their high schools for college credit. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
   </si>
   <si>
-    <t>2012 annual number of FTE executive staff who directly support the instructional function as administrators (e.g. Chief Academic Officer, Vice President of Academic Affairs, Deans, Provosts or other instructional leadership.)</t>
-  </si>
-  <si>
     <t>Fiscal year 2012-2013 salaries and benefits for all full-time credit instructional faculty in the academic unit.</t>
   </si>
   <si>
@@ -5253,9 +5250,6 @@
     <t>Enter the number of student credit hours taught by full-time faculty in the academic unit in the 2013 academic year. This should be the number of credit hours for a course times the number of students enrolled in the course (include students who received a grade of W). For example, a 3 credit hour course with 30 enrolled students would generate 90 student credit hours. Exclude high school students taking classes taught by high school faculty in their high schools for college credit. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
   </si>
   <si>
-    <t>Enter the 2012 annual FTE credit instructional clerical and other professional support staff. The calculation for FTE = (number of full-time staff) + (part-time staff hours / 2080)</t>
-  </si>
-  <si>
     <t>Full-time equivalent (FTE) faculty will equal instructor credit hours taught by all full-time credit faculty in the academic unit in the 2013 academic year divided by 15. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
   </si>
   <si>
@@ -5263,6 +5257,12 @@
   </si>
   <si>
     <t>Enter the number of student credit hours taught by part-time faculty or adjuncts in the academic unit in the 2013 academic year. This should be the number of credit hours for a course times the number of students enrolled in the course (include students who received a grade of W). For example, a 3 credit hour course with 30 enrolled students would generate 90 student credit hours. Exclude high school students taking classes taught by high school faculty in their high schools for college credit. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
+  </si>
+  <si>
+    <t>2013 annual number of FTE executive staff who directly support the instructional function as administrators (e.g. Chief Academic Officer, Vice President of Academic Affairs, Deans, Provosts or other instructional leadership.)</t>
+  </si>
+  <si>
+    <t>Enter the 2013 annual FTE credit instructional clerical and other professional support staff. The calculation for FTE = (number of full-time staff) + (part-time staff hours / 2080)</t>
   </si>
 </sst>
 </file>
@@ -6362,28 +6362,26 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="33" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
@@ -6399,16 +6397,18 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="15"/>
     </xf>
@@ -7342,8 +7342,8 @@
   </sheetPr>
   <dimension ref="A1:X509"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7359,11 +7359,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="9" customFormat="1" ht="66.5" customHeight="1">
-      <c r="A1" s="230" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="230"/>
-      <c r="C1" s="230"/>
+      <c r="A1" s="243" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
       <c r="D1" s="42"/>
       <c r="E1" s="42"/>
       <c r="F1" s="10"/>
@@ -7396,21 +7396,21 @@
       <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:24" s="11" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A4" s="234" t="s">
+      <c r="A4" s="245" t="s">
         <v>521</v>
       </c>
-      <c r="B4" s="235"/>
-      <c r="C4" s="235"/>
+      <c r="B4" s="246"/>
+      <c r="C4" s="246"/>
       <c r="D4" s="190"/>
       <c r="E4" s="190"/>
       <c r="F4" s="10"/>
     </row>
     <row r="6" spans="1:24" ht="48.75" customHeight="1">
-      <c r="A6" s="233" t="s">
+      <c r="A6" s="244" t="s">
         <v>522</v>
       </c>
-      <c r="B6" s="233"/>
-      <c r="C6" s="233"/>
+      <c r="B6" s="244"/>
+      <c r="C6" s="244"/>
       <c r="D6" s="191"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
@@ -7441,11 +7441,11 @@
       <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:24" s="171" customFormat="1" ht="40" customHeight="1">
-      <c r="A8" s="236" t="s">
+      <c r="A8" s="234" t="s">
         <v>685</v>
       </c>
-      <c r="B8" s="237"/>
-      <c r="C8" s="237"/>
+      <c r="B8" s="235"/>
+      <c r="C8" s="235"/>
       <c r="D8" s="42"/>
       <c r="E8" s="42"/>
       <c r="F8" s="18"/>
@@ -7470,7 +7470,7 @@
     </row>
     <row r="9" spans="1:24" s="64" customFormat="1" ht="24" customHeight="1">
       <c r="A9" s="176" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B9" s="71"/>
       <c r="C9" s="70"/>
@@ -7553,11 +7553,11 @@
       <c r="X11" s="69"/>
     </row>
     <row r="12" spans="1:24" s="64" customFormat="1" ht="18" customHeight="1">
-      <c r="A12" s="231" t="s">
+      <c r="A12" s="232" t="s">
         <v>456</v>
       </c>
-      <c r="B12" s="232"/>
-      <c r="C12" s="232"/>
+      <c r="B12" s="233"/>
+      <c r="C12" s="233"/>
       <c r="D12" s="192"/>
       <c r="E12" s="192"/>
       <c r="F12" s="69"/>
@@ -7645,7 +7645,7 @@
     </row>
     <row r="16" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A16" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B16" s="80"/>
       <c r="C16" s="48" t="s">
@@ -7660,7 +7660,7 @@
     </row>
     <row r="17" spans="1:24" ht="39" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B17" s="81"/>
       <c r="C17" s="48" t="s">
@@ -7698,7 +7698,7 @@
     </row>
     <row r="20" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A20" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B20" s="80"/>
       <c r="C20" s="49" t="s">
@@ -7713,7 +7713,7 @@
     </row>
     <row r="21" spans="1:24" ht="52.5" customHeight="1" thickBot="1">
       <c r="A21" s="229" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="B21" s="81"/>
       <c r="C21" s="49" t="s">
@@ -7771,7 +7771,7 @@
     </row>
     <row r="24" spans="1:24" ht="49" thickBot="1">
       <c r="A24" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B24" s="80"/>
       <c r="C24" s="227" t="s">
@@ -7786,11 +7786,11 @@
     </row>
     <row r="25" spans="1:24" ht="47.25" customHeight="1" thickBot="1">
       <c r="A25" s="75" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B25" s="81"/>
       <c r="C25" s="65" t="s">
-        <v>987</v>
+        <v>1003</v>
       </c>
       <c r="D25" s="42" t="s">
         <v>724</v>
@@ -7829,7 +7829,7 @@
     </row>
     <row r="27" spans="1:24" ht="48" customHeight="1" thickBot="1">
       <c r="A27" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B27" s="80"/>
       <c r="C27" s="49" t="s">
@@ -7844,11 +7844,11 @@
     </row>
     <row r="28" spans="1:24" ht="46.5" customHeight="1" thickBot="1">
       <c r="A28" s="75" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B28" s="81"/>
       <c r="C28" s="49" t="s">
-        <v>1001</v>
+        <v>1004</v>
       </c>
       <c r="D28" s="42" t="s">
         <v>539</v>
@@ -7859,7 +7859,7 @@
     </row>
     <row r="29" spans="1:24" ht="49.5" customHeight="1" thickBot="1">
       <c r="A29" s="78" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B29" s="80"/>
       <c r="C29" s="48" t="s">
@@ -7881,11 +7881,11 @@
       <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:24" ht="40" customHeight="1">
-      <c r="A31" s="236" t="s">
+      <c r="A31" s="234" t="s">
         <v>457</v>
       </c>
-      <c r="B31" s="237"/>
-      <c r="C31" s="237"/>
+      <c r="B31" s="235"/>
+      <c r="C31" s="235"/>
       <c r="F31" s="18"/>
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
@@ -7908,7 +7908,7 @@
     </row>
     <row r="32" spans="1:24" s="64" customFormat="1" ht="24" customHeight="1">
       <c r="A32" s="176" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B32" s="71"/>
       <c r="C32" s="70"/>
@@ -8217,10 +8217,10 @@
       <c r="F49" s="10"/>
     </row>
     <row r="50" spans="1:24" ht="40" customHeight="1">
-      <c r="A50" s="236" t="s">
+      <c r="A50" s="234" t="s">
         <v>470</v>
       </c>
-      <c r="B50" s="237"/>
+      <c r="B50" s="235"/>
       <c r="C50" s="59"/>
       <c r="F50" s="18"/>
       <c r="G50" s="18"/>
@@ -8327,11 +8327,11 @@
       <c r="X53" s="69"/>
     </row>
     <row r="54" spans="1:24" s="64" customFormat="1" ht="18" customHeight="1">
-      <c r="A54" s="231" t="s">
+      <c r="A54" s="232" t="s">
         <v>456</v>
       </c>
-      <c r="B54" s="232"/>
-      <c r="C54" s="232"/>
+      <c r="B54" s="233"/>
+      <c r="C54" s="233"/>
       <c r="D54" s="42"/>
       <c r="E54" s="192"/>
       <c r="F54" s="69"/>
@@ -8384,8 +8384,8 @@
       <c r="A56" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="243"/>
-      <c r="C56" s="244"/>
+      <c r="B56" s="236"/>
+      <c r="C56" s="237"/>
       <c r="F56" s="32"/>
       <c r="G56" s="32"/>
       <c r="H56" s="32"/>
@@ -9354,10 +9354,10 @@
       <c r="F124" s="10"/>
     </row>
     <row r="125" spans="1:24" s="171" customFormat="1" ht="40" customHeight="1">
-      <c r="A125" s="236" t="s">
+      <c r="A125" s="234" t="s">
         <v>689</v>
       </c>
-      <c r="B125" s="237"/>
+      <c r="B125" s="235"/>
       <c r="C125" s="59"/>
       <c r="D125" s="42"/>
       <c r="E125" s="42"/>
@@ -9438,11 +9438,11 @@
       <c r="X127" s="69"/>
     </row>
     <row r="128" spans="1:24" s="64" customFormat="1" ht="18" customHeight="1">
-      <c r="A128" s="231" t="s">
+      <c r="A128" s="232" t="s">
         <v>456</v>
       </c>
-      <c r="B128" s="232"/>
-      <c r="C128" s="232"/>
+      <c r="B128" s="233"/>
+      <c r="C128" s="233"/>
       <c r="D128" s="33"/>
       <c r="E128" s="192"/>
       <c r="F128" s="69"/>
@@ -9495,8 +9495,8 @@
       <c r="A130" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="B130" s="243"/>
-      <c r="C130" s="244"/>
+      <c r="B130" s="236"/>
+      <c r="C130" s="237"/>
       <c r="D130" s="33"/>
       <c r="F130" s="14"/>
       <c r="G130" s="14"/>
@@ -9581,8 +9581,8 @@
       <c r="A136" s="103" t="s">
         <v>71</v>
       </c>
-      <c r="B136" s="243"/>
-      <c r="C136" s="244"/>
+      <c r="B136" s="236"/>
+      <c r="C136" s="237"/>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
       <c r="H136" s="14"/>
@@ -9748,10 +9748,10 @@
       <c r="F147" s="10"/>
     </row>
     <row r="148" spans="1:24" s="61" customFormat="1" ht="40" customHeight="1">
-      <c r="A148" s="236" t="s">
+      <c r="A148" s="234" t="s">
         <v>476</v>
       </c>
-      <c r="B148" s="237"/>
+      <c r="B148" s="235"/>
       <c r="C148" s="59"/>
       <c r="D148" s="42"/>
       <c r="E148" s="42"/>
@@ -9804,11 +9804,11 @@
       <c r="X149" s="69"/>
     </row>
     <row r="150" spans="1:24" s="64" customFormat="1" ht="24" customHeight="1">
-      <c r="A150" s="231" t="s">
+      <c r="A150" s="232" t="s">
         <v>478</v>
       </c>
-      <c r="B150" s="232"/>
-      <c r="C150" s="232"/>
+      <c r="B150" s="233"/>
+      <c r="C150" s="233"/>
       <c r="D150" s="42"/>
       <c r="E150" s="192"/>
       <c r="F150" s="69"/>
@@ -9858,10 +9858,10 @@
       <c r="X151" s="97"/>
     </row>
     <row r="152" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A152" s="245" t="s">
+      <c r="A152" s="230" t="s">
         <v>479</v>
       </c>
-      <c r="B152" s="246"/>
+      <c r="B152" s="231"/>
       <c r="C152" s="107"/>
       <c r="D152" s="42"/>
       <c r="E152" s="42"/>
@@ -9945,10 +9945,10 @@
       <c r="H156" s="14"/>
     </row>
     <row r="157" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A157" s="245" t="s">
+      <c r="A157" s="230" t="s">
         <v>480</v>
       </c>
-      <c r="B157" s="246"/>
+      <c r="B157" s="231"/>
       <c r="C157" s="107"/>
       <c r="D157" s="42" t="s">
         <v>740</v>
@@ -10201,10 +10201,10 @@
       <c r="H172" s="14"/>
     </row>
     <row r="173" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A173" s="245" t="s">
+      <c r="A173" s="230" t="s">
         <v>481</v>
       </c>
-      <c r="B173" s="246"/>
+      <c r="B173" s="231"/>
       <c r="C173" s="107"/>
       <c r="D173" s="42"/>
       <c r="E173" s="42"/>
@@ -10361,10 +10361,10 @@
       <c r="H183" s="14"/>
     </row>
     <row r="184" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A184" s="245" t="s">
+      <c r="A184" s="230" t="s">
         <v>491</v>
       </c>
-      <c r="B184" s="246"/>
+      <c r="B184" s="231"/>
       <c r="C184" s="107"/>
       <c r="D184" s="42"/>
       <c r="E184" s="42"/>
@@ -10431,10 +10431,10 @@
       <c r="H187" s="14"/>
     </row>
     <row r="188" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A188" s="245" t="s">
+      <c r="A188" s="230" t="s">
         <v>492</v>
       </c>
-      <c r="B188" s="246"/>
+      <c r="B188" s="231"/>
       <c r="C188" s="107"/>
       <c r="D188" s="42"/>
       <c r="E188" s="42"/>
@@ -10534,10 +10534,10 @@
       <c r="H194" s="14"/>
     </row>
     <row r="195" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A195" s="245" t="s">
+      <c r="A195" s="230" t="s">
         <v>115</v>
       </c>
-      <c r="B195" s="246"/>
+      <c r="B195" s="231"/>
       <c r="C195" s="107"/>
       <c r="D195" s="42"/>
       <c r="E195" s="42"/>
@@ -10675,10 +10675,10 @@
       <c r="H202" s="42"/>
     </row>
     <row r="203" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A203" s="245" t="s">
+      <c r="A203" s="230" t="s">
         <v>502</v>
       </c>
-      <c r="B203" s="246"/>
+      <c r="B203" s="231"/>
       <c r="C203" s="107"/>
       <c r="D203" s="42"/>
       <c r="E203" s="42"/>
@@ -10779,10 +10779,10 @@
       <c r="F208" s="10"/>
     </row>
     <row r="209" spans="1:24" s="61" customFormat="1" ht="40" customHeight="1">
-      <c r="A209" s="236" t="s">
+      <c r="A209" s="234" t="s">
         <v>503</v>
       </c>
-      <c r="B209" s="237"/>
+      <c r="B209" s="235"/>
       <c r="C209" s="59"/>
       <c r="D209" s="42"/>
       <c r="E209" s="42"/>
@@ -10868,8 +10868,8 @@
       <c r="A212" s="238" t="s">
         <v>706</v>
       </c>
-      <c r="B212" s="232"/>
-      <c r="C212" s="232"/>
+      <c r="B212" s="233"/>
+      <c r="C212" s="233"/>
       <c r="D212" s="42"/>
       <c r="E212" s="192"/>
       <c r="F212" s="69"/>
@@ -10893,10 +10893,10 @@
       <c r="X212" s="69"/>
     </row>
     <row r="213" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A213" s="245" t="s">
+      <c r="A213" s="230" t="s">
         <v>504</v>
       </c>
-      <c r="B213" s="246"/>
+      <c r="B213" s="231"/>
       <c r="C213" s="107"/>
       <c r="D213" s="42"/>
       <c r="E213" s="42"/>
@@ -10982,10 +10982,10 @@
       <c r="H217" s="14"/>
     </row>
     <row r="218" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A218" s="245" t="s">
+      <c r="A218" s="230" t="s">
         <v>504</v>
       </c>
-      <c r="B218" s="246"/>
+      <c r="B218" s="231"/>
       <c r="C218" s="107"/>
       <c r="D218" s="42"/>
       <c r="E218" s="42"/>
@@ -11070,10 +11070,10 @@
       <c r="H222" s="14"/>
     </row>
     <row r="223" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A223" s="245" t="s">
+      <c r="A223" s="230" t="s">
         <v>504</v>
       </c>
-      <c r="B223" s="246"/>
+      <c r="B223" s="231"/>
       <c r="C223" s="107"/>
       <c r="D223" s="42"/>
       <c r="E223" s="42"/>
@@ -11153,10 +11153,10 @@
       <c r="H227" s="14"/>
     </row>
     <row r="228" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A228" s="245" t="s">
+      <c r="A228" s="230" t="s">
         <v>504</v>
       </c>
-      <c r="B228" s="246"/>
+      <c r="B228" s="231"/>
       <c r="C228" s="107"/>
       <c r="D228" s="42"/>
       <c r="E228" s="42"/>
@@ -15766,6 +15766,21 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="31">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A212:C212"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A125:B125"/>
     <mergeCell ref="A213:B213"/>
     <mergeCell ref="A218:B218"/>
     <mergeCell ref="A228:B228"/>
@@ -15782,21 +15797,6 @@
     <mergeCell ref="A188:B188"/>
     <mergeCell ref="A195:B195"/>
     <mergeCell ref="A203:B203"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A212:C212"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A8:C8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A36" location="'Move or Copy'!A1" display="Link to Move or Copy"/>
@@ -15947,7 +15947,7 @@
     </row>
     <row r="7" spans="1:25" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -16050,12 +16050,12 @@
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -16065,12 +16065,12 @@
     </row>
     <row r="14" spans="1:25" ht="48" customHeight="1" thickBot="1">
       <c r="A14" s="75" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -16085,7 +16085,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -16103,12 +16103,12 @@
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -16118,12 +16118,12 @@
     </row>
     <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -16138,7 +16138,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -16213,8 +16213,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -16576,7 +16576,7 @@
     </row>
     <row r="7" spans="1:25" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -16632,7 +16632,7 @@
     </row>
     <row r="9" spans="1:25" s="130" customFormat="1" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="131" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B9" s="127"/>
       <c r="C9" s="127"/>
@@ -16679,12 +16679,12 @@
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -16699,7 +16699,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -16714,7 +16714,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -16732,12 +16732,12 @@
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -16752,7 +16752,7 @@
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -16767,7 +16767,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -16842,8 +16842,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -17207,7 +17207,7 @@
       <c r="W5" s="3"/>
     </row>
     <row r="6" spans="1:25" s="171" customFormat="1" ht="36" customHeight="1">
-      <c r="A6" s="236" t="s">
+      <c r="A6" s="234" t="s">
         <v>701</v>
       </c>
       <c r="B6" s="254"/>
@@ -17236,7 +17236,7 @@
     </row>
     <row r="7" spans="1:25" s="62" customFormat="1" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -17341,12 +17341,12 @@
     </row>
     <row r="13" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="14"/>
@@ -17356,12 +17356,12 @@
     </row>
     <row r="14" spans="1:25" s="1" customFormat="1" ht="48" customHeight="1" thickBot="1">
       <c r="A14" s="75" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="180" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="14"/>
@@ -17376,7 +17376,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="180" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="13"/>
@@ -17398,12 +17398,12 @@
     </row>
     <row r="17" spans="1:24" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="14"/>
@@ -17413,12 +17413,12 @@
     </row>
     <row r="18" spans="1:24" s="1" customFormat="1" ht="55.5" customHeight="1" thickBot="1">
       <c r="A18" s="75" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="135"/>
       <c r="D18" s="180" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="14"/>
@@ -17433,7 +17433,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="66"/>
       <c r="D19" s="140" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
@@ -17507,8 +17507,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -18176,7 +18176,7 @@
     </row>
     <row r="7" spans="1:25" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -18279,12 +18279,12 @@
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -18294,12 +18294,12 @@
     </row>
     <row r="14" spans="1:25" ht="48" customHeight="1" thickBot="1">
       <c r="A14" s="76" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="180" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -18314,7 +18314,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="180" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -18332,12 +18332,12 @@
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -18347,12 +18347,12 @@
     </row>
     <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="180" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -18367,7 +18367,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -18442,8 +18442,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -18802,7 +18802,7 @@
     </row>
     <row r="7" spans="1:25" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -18905,12 +18905,12 @@
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -18920,12 +18920,12 @@
     </row>
     <row r="14" spans="1:25" ht="48" customHeight="1" thickBot="1">
       <c r="A14" s="76" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -18940,7 +18940,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -18958,12 +18958,12 @@
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -18973,12 +18973,12 @@
     </row>
     <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -18993,7 +18993,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -19068,8 +19068,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -19428,7 +19428,7 @@
     </row>
     <row r="7" spans="1:25" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -19531,12 +19531,12 @@
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -19546,12 +19546,12 @@
     </row>
     <row r="14" spans="1:25" ht="48" customHeight="1" thickBot="1">
       <c r="A14" s="76" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -19566,7 +19566,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42" t="s">
@@ -19586,12 +19586,12 @@
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -19601,12 +19601,12 @@
     </row>
     <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -19621,7 +19621,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -19696,8 +19696,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -20059,7 +20059,7 @@
     </row>
     <row r="7" spans="1:25" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -20164,12 +20164,12 @@
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -20179,12 +20179,12 @@
     </row>
     <row r="14" spans="1:25" ht="48" customHeight="1" thickBot="1">
       <c r="A14" s="76" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -20199,7 +20199,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -20217,12 +20217,12 @@
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -20232,12 +20232,12 @@
     </row>
     <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -20252,7 +20252,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -20327,8 +20327,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -20690,7 +20690,7 @@
     </row>
     <row r="7" spans="1:25" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -20793,12 +20793,12 @@
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -20808,12 +20808,12 @@
     </row>
     <row r="14" spans="1:25" ht="48" customHeight="1" thickBot="1">
       <c r="A14" s="76" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -20828,7 +20828,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -20846,12 +20846,12 @@
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -20861,12 +20861,12 @@
     </row>
     <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -20881,7 +20881,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -20956,8 +20956,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -21319,7 +21319,7 @@
     </row>
     <row r="7" spans="1:25" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -21375,7 +21375,7 @@
     </row>
     <row r="9" spans="1:25" s="130" customFormat="1" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="131" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B9" s="127"/>
       <c r="C9" s="127"/>
@@ -21422,12 +21422,12 @@
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -21437,12 +21437,12 @@
     </row>
     <row r="14" spans="1:25" ht="48" customHeight="1" thickBot="1">
       <c r="A14" s="76" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -21457,7 +21457,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -21475,12 +21475,12 @@
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -21490,12 +21490,12 @@
     </row>
     <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -21510,7 +21510,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -21585,8 +21585,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -21948,7 +21948,7 @@
     </row>
     <row r="7" spans="1:25" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -22004,7 +22004,7 @@
     </row>
     <row r="9" spans="1:25" s="130" customFormat="1" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="131" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B9" s="127"/>
       <c r="C9" s="127"/>
@@ -22051,12 +22051,12 @@
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -22066,12 +22066,12 @@
     </row>
     <row r="14" spans="1:25" ht="48" customHeight="1" thickBot="1">
       <c r="A14" s="76" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -22086,7 +22086,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -22104,12 +22104,12 @@
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -22119,12 +22119,12 @@
     </row>
     <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -22139,7 +22139,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -22214,8 +22214,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>

</xml_diff>

<commit_message>
update data label in excel
</commit_message>
<xml_diff>
--- a/data/imports/mrss-export.xlsx
+++ b/data/imports/mrss-export.xlsx
@@ -5219,9 +5219,6 @@
     <t>Number of Academic Year 2013 FTE Faculty/Adjuncts</t>
   </si>
   <si>
-    <t>2012 Annual Number of FTE Staff</t>
-  </si>
-  <si>
     <t>FY 2012/13 Non-labor Operating Costs</t>
   </si>
   <si>
@@ -5263,6 +5260,9 @@
   </si>
   <si>
     <t>Enter the 2013 annual FTE credit instructional clerical and other professional support staff. The calculation for FTE = (number of full-time staff) + (part-time staff hours / 2080)</t>
+  </si>
+  <si>
+    <t>2013 Annual Number of FTE Staff</t>
   </si>
 </sst>
 </file>
@@ -6362,26 +6362,28 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="33" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
@@ -6397,18 +6399,16 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="15"/>
     </xf>
@@ -7343,7 +7343,7 @@
   <dimension ref="A1:X509"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7359,11 +7359,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="9" customFormat="1" ht="66.5" customHeight="1">
-      <c r="A1" s="243" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="243"/>
-      <c r="C1" s="243"/>
+      <c r="A1" s="230" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="230"/>
+      <c r="C1" s="230"/>
       <c r="D1" s="42"/>
       <c r="E1" s="42"/>
       <c r="F1" s="10"/>
@@ -7396,21 +7396,21 @@
       <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:24" s="11" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A4" s="245" t="s">
+      <c r="A4" s="234" t="s">
         <v>521</v>
       </c>
-      <c r="B4" s="246"/>
-      <c r="C4" s="246"/>
+      <c r="B4" s="235"/>
+      <c r="C4" s="235"/>
       <c r="D4" s="190"/>
       <c r="E4" s="190"/>
       <c r="F4" s="10"/>
     </row>
     <row r="6" spans="1:24" ht="48.75" customHeight="1">
-      <c r="A6" s="244" t="s">
+      <c r="A6" s="233" t="s">
         <v>522</v>
       </c>
-      <c r="B6" s="244"/>
-      <c r="C6" s="244"/>
+      <c r="B6" s="233"/>
+      <c r="C6" s="233"/>
       <c r="D6" s="191"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
@@ -7441,11 +7441,11 @@
       <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:24" s="171" customFormat="1" ht="40" customHeight="1">
-      <c r="A8" s="234" t="s">
+      <c r="A8" s="236" t="s">
         <v>685</v>
       </c>
-      <c r="B8" s="235"/>
-      <c r="C8" s="235"/>
+      <c r="B8" s="237"/>
+      <c r="C8" s="237"/>
       <c r="D8" s="42"/>
       <c r="E8" s="42"/>
       <c r="F8" s="18"/>
@@ -7553,11 +7553,11 @@
       <c r="X11" s="69"/>
     </row>
     <row r="12" spans="1:24" s="64" customFormat="1" ht="18" customHeight="1">
-      <c r="A12" s="232" t="s">
+      <c r="A12" s="231" t="s">
         <v>456</v>
       </c>
-      <c r="B12" s="233"/>
-      <c r="C12" s="233"/>
+      <c r="B12" s="232"/>
+      <c r="C12" s="232"/>
       <c r="D12" s="192"/>
       <c r="E12" s="192"/>
       <c r="F12" s="69"/>
@@ -7786,11 +7786,11 @@
     </row>
     <row r="25" spans="1:24" ht="47.25" customHeight="1" thickBot="1">
       <c r="A25" s="75" t="s">
-        <v>996</v>
+        <v>1004</v>
       </c>
       <c r="B25" s="81"/>
       <c r="C25" s="65" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D25" s="42" t="s">
         <v>724</v>
@@ -7844,11 +7844,11 @@
     </row>
     <row r="28" spans="1:24" ht="46.5" customHeight="1" thickBot="1">
       <c r="A28" s="75" t="s">
-        <v>996</v>
+        <v>1004</v>
       </c>
       <c r="B28" s="81"/>
       <c r="C28" s="49" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="D28" s="42" t="s">
         <v>539</v>
@@ -7859,7 +7859,7 @@
     </row>
     <row r="29" spans="1:24" ht="49.5" customHeight="1" thickBot="1">
       <c r="A29" s="78" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B29" s="80"/>
       <c r="C29" s="48" t="s">
@@ -7881,11 +7881,11 @@
       <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:24" ht="40" customHeight="1">
-      <c r="A31" s="234" t="s">
+      <c r="A31" s="236" t="s">
         <v>457</v>
       </c>
-      <c r="B31" s="235"/>
-      <c r="C31" s="235"/>
+      <c r="B31" s="237"/>
+      <c r="C31" s="237"/>
       <c r="F31" s="18"/>
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
@@ -8217,10 +8217,10 @@
       <c r="F49" s="10"/>
     </row>
     <row r="50" spans="1:24" ht="40" customHeight="1">
-      <c r="A50" s="234" t="s">
+      <c r="A50" s="236" t="s">
         <v>470</v>
       </c>
-      <c r="B50" s="235"/>
+      <c r="B50" s="237"/>
       <c r="C50" s="59"/>
       <c r="F50" s="18"/>
       <c r="G50" s="18"/>
@@ -8327,11 +8327,11 @@
       <c r="X53" s="69"/>
     </row>
     <row r="54" spans="1:24" s="64" customFormat="1" ht="18" customHeight="1">
-      <c r="A54" s="232" t="s">
+      <c r="A54" s="231" t="s">
         <v>456</v>
       </c>
-      <c r="B54" s="233"/>
-      <c r="C54" s="233"/>
+      <c r="B54" s="232"/>
+      <c r="C54" s="232"/>
       <c r="D54" s="42"/>
       <c r="E54" s="192"/>
       <c r="F54" s="69"/>
@@ -8384,8 +8384,8 @@
       <c r="A56" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="236"/>
-      <c r="C56" s="237"/>
+      <c r="B56" s="243"/>
+      <c r="C56" s="244"/>
       <c r="F56" s="32"/>
       <c r="G56" s="32"/>
       <c r="H56" s="32"/>
@@ -9354,10 +9354,10 @@
       <c r="F124" s="10"/>
     </row>
     <row r="125" spans="1:24" s="171" customFormat="1" ht="40" customHeight="1">
-      <c r="A125" s="234" t="s">
+      <c r="A125" s="236" t="s">
         <v>689</v>
       </c>
-      <c r="B125" s="235"/>
+      <c r="B125" s="237"/>
       <c r="C125" s="59"/>
       <c r="D125" s="42"/>
       <c r="E125" s="42"/>
@@ -9438,11 +9438,11 @@
       <c r="X127" s="69"/>
     </row>
     <row r="128" spans="1:24" s="64" customFormat="1" ht="18" customHeight="1">
-      <c r="A128" s="232" t="s">
+      <c r="A128" s="231" t="s">
         <v>456</v>
       </c>
-      <c r="B128" s="233"/>
-      <c r="C128" s="233"/>
+      <c r="B128" s="232"/>
+      <c r="C128" s="232"/>
       <c r="D128" s="33"/>
       <c r="E128" s="192"/>
       <c r="F128" s="69"/>
@@ -9495,8 +9495,8 @@
       <c r="A130" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="B130" s="236"/>
-      <c r="C130" s="237"/>
+      <c r="B130" s="243"/>
+      <c r="C130" s="244"/>
       <c r="D130" s="33"/>
       <c r="F130" s="14"/>
       <c r="G130" s="14"/>
@@ -9581,8 +9581,8 @@
       <c r="A136" s="103" t="s">
         <v>71</v>
       </c>
-      <c r="B136" s="236"/>
-      <c r="C136" s="237"/>
+      <c r="B136" s="243"/>
+      <c r="C136" s="244"/>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
       <c r="H136" s="14"/>
@@ -9748,10 +9748,10 @@
       <c r="F147" s="10"/>
     </row>
     <row r="148" spans="1:24" s="61" customFormat="1" ht="40" customHeight="1">
-      <c r="A148" s="234" t="s">
+      <c r="A148" s="236" t="s">
         <v>476</v>
       </c>
-      <c r="B148" s="235"/>
+      <c r="B148" s="237"/>
       <c r="C148" s="59"/>
       <c r="D148" s="42"/>
       <c r="E148" s="42"/>
@@ -9804,11 +9804,11 @@
       <c r="X149" s="69"/>
     </row>
     <row r="150" spans="1:24" s="64" customFormat="1" ht="24" customHeight="1">
-      <c r="A150" s="232" t="s">
+      <c r="A150" s="231" t="s">
         <v>478</v>
       </c>
-      <c r="B150" s="233"/>
-      <c r="C150" s="233"/>
+      <c r="B150" s="232"/>
+      <c r="C150" s="232"/>
       <c r="D150" s="42"/>
       <c r="E150" s="192"/>
       <c r="F150" s="69"/>
@@ -9858,10 +9858,10 @@
       <c r="X151" s="97"/>
     </row>
     <row r="152" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A152" s="230" t="s">
+      <c r="A152" s="245" t="s">
         <v>479</v>
       </c>
-      <c r="B152" s="231"/>
+      <c r="B152" s="246"/>
       <c r="C152" s="107"/>
       <c r="D152" s="42"/>
       <c r="E152" s="42"/>
@@ -9945,10 +9945,10 @@
       <c r="H156" s="14"/>
     </row>
     <row r="157" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A157" s="230" t="s">
+      <c r="A157" s="245" t="s">
         <v>480</v>
       </c>
-      <c r="B157" s="231"/>
+      <c r="B157" s="246"/>
       <c r="C157" s="107"/>
       <c r="D157" s="42" t="s">
         <v>740</v>
@@ -10201,10 +10201,10 @@
       <c r="H172" s="14"/>
     </row>
     <row r="173" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A173" s="230" t="s">
+      <c r="A173" s="245" t="s">
         <v>481</v>
       </c>
-      <c r="B173" s="231"/>
+      <c r="B173" s="246"/>
       <c r="C173" s="107"/>
       <c r="D173" s="42"/>
       <c r="E173" s="42"/>
@@ -10361,10 +10361,10 @@
       <c r="H183" s="14"/>
     </row>
     <row r="184" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A184" s="230" t="s">
+      <c r="A184" s="245" t="s">
         <v>491</v>
       </c>
-      <c r="B184" s="231"/>
+      <c r="B184" s="246"/>
       <c r="C184" s="107"/>
       <c r="D184" s="42"/>
       <c r="E184" s="42"/>
@@ -10431,10 +10431,10 @@
       <c r="H187" s="14"/>
     </row>
     <row r="188" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A188" s="230" t="s">
+      <c r="A188" s="245" t="s">
         <v>492</v>
       </c>
-      <c r="B188" s="231"/>
+      <c r="B188" s="246"/>
       <c r="C188" s="107"/>
       <c r="D188" s="42"/>
       <c r="E188" s="42"/>
@@ -10534,10 +10534,10 @@
       <c r="H194" s="14"/>
     </row>
     <row r="195" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A195" s="230" t="s">
+      <c r="A195" s="245" t="s">
         <v>115</v>
       </c>
-      <c r="B195" s="231"/>
+      <c r="B195" s="246"/>
       <c r="C195" s="107"/>
       <c r="D195" s="42"/>
       <c r="E195" s="42"/>
@@ -10675,10 +10675,10 @@
       <c r="H202" s="42"/>
     </row>
     <row r="203" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A203" s="230" t="s">
+      <c r="A203" s="245" t="s">
         <v>502</v>
       </c>
-      <c r="B203" s="231"/>
+      <c r="B203" s="246"/>
       <c r="C203" s="107"/>
       <c r="D203" s="42"/>
       <c r="E203" s="42"/>
@@ -10779,10 +10779,10 @@
       <c r="F208" s="10"/>
     </row>
     <row r="209" spans="1:24" s="61" customFormat="1" ht="40" customHeight="1">
-      <c r="A209" s="234" t="s">
+      <c r="A209" s="236" t="s">
         <v>503</v>
       </c>
-      <c r="B209" s="235"/>
+      <c r="B209" s="237"/>
       <c r="C209" s="59"/>
       <c r="D209" s="42"/>
       <c r="E209" s="42"/>
@@ -10868,8 +10868,8 @@
       <c r="A212" s="238" t="s">
         <v>706</v>
       </c>
-      <c r="B212" s="233"/>
-      <c r="C212" s="233"/>
+      <c r="B212" s="232"/>
+      <c r="C212" s="232"/>
       <c r="D212" s="42"/>
       <c r="E212" s="192"/>
       <c r="F212" s="69"/>
@@ -10893,10 +10893,10 @@
       <c r="X212" s="69"/>
     </row>
     <row r="213" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A213" s="230" t="s">
+      <c r="A213" s="245" t="s">
         <v>504</v>
       </c>
-      <c r="B213" s="231"/>
+      <c r="B213" s="246"/>
       <c r="C213" s="107"/>
       <c r="D213" s="42"/>
       <c r="E213" s="42"/>
@@ -10982,10 +10982,10 @@
       <c r="H217" s="14"/>
     </row>
     <row r="218" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A218" s="230" t="s">
+      <c r="A218" s="245" t="s">
         <v>504</v>
       </c>
-      <c r="B218" s="231"/>
+      <c r="B218" s="246"/>
       <c r="C218" s="107"/>
       <c r="D218" s="42"/>
       <c r="E218" s="42"/>
@@ -11070,10 +11070,10 @@
       <c r="H222" s="14"/>
     </row>
     <row r="223" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A223" s="230" t="s">
+      <c r="A223" s="245" t="s">
         <v>504</v>
       </c>
-      <c r="B223" s="231"/>
+      <c r="B223" s="246"/>
       <c r="C223" s="107"/>
       <c r="D223" s="42"/>
       <c r="E223" s="42"/>
@@ -11153,10 +11153,10 @@
       <c r="H227" s="14"/>
     </row>
     <row r="228" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A228" s="230" t="s">
+      <c r="A228" s="245" t="s">
         <v>504</v>
       </c>
-      <c r="B228" s="231"/>
+      <c r="B228" s="246"/>
       <c r="C228" s="107"/>
       <c r="D228" s="42"/>
       <c r="E228" s="42"/>
@@ -15766,21 +15766,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="31">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A212:C212"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A125:B125"/>
     <mergeCell ref="A213:B213"/>
     <mergeCell ref="A218:B218"/>
     <mergeCell ref="A228:B228"/>
@@ -15797,6 +15782,21 @@
     <mergeCell ref="A188:B188"/>
     <mergeCell ref="A195:B195"/>
     <mergeCell ref="A203:B203"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A212:C212"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A8:C8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A36" location="'Move or Copy'!A1" display="Link to Move or Copy"/>
@@ -16070,7 +16070,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -16085,7 +16085,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -16123,7 +16123,7 @@
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -16138,7 +16138,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -16213,8 +16213,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -16699,7 +16699,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -16714,7 +16714,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -16752,7 +16752,7 @@
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -16767,7 +16767,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -16842,8 +16842,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -17207,7 +17207,7 @@
       <c r="W5" s="3"/>
     </row>
     <row r="6" spans="1:25" s="171" customFormat="1" ht="36" customHeight="1">
-      <c r="A6" s="234" t="s">
+      <c r="A6" s="236" t="s">
         <v>701</v>
       </c>
       <c r="B6" s="254"/>
@@ -17361,7 +17361,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="180" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="14"/>
@@ -17376,7 +17376,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="180" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="13"/>
@@ -17418,7 +17418,7 @@
       <c r="B18" s="134"/>
       <c r="C18" s="135"/>
       <c r="D18" s="180" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="14"/>
@@ -17433,7 +17433,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="66"/>
       <c r="D19" s="140" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
@@ -17507,8 +17507,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -18299,7 +18299,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="180" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -18314,7 +18314,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="180" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -18352,7 +18352,7 @@
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="180" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -18367,7 +18367,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -18442,8 +18442,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -18925,7 +18925,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -18940,7 +18940,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -18978,7 +18978,7 @@
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -18993,7 +18993,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -19068,8 +19068,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -19551,7 +19551,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -19566,7 +19566,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42" t="s">
@@ -19606,7 +19606,7 @@
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -19621,7 +19621,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -19696,8 +19696,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -20184,7 +20184,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -20199,7 +20199,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -20237,7 +20237,7 @@
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -20252,7 +20252,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -20327,8 +20327,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -20813,7 +20813,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -20828,7 +20828,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -20866,7 +20866,7 @@
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -20881,7 +20881,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -20956,8 +20956,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -21442,7 +21442,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -21457,7 +21457,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -21495,7 +21495,7 @@
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -21510,7 +21510,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -21585,8 +21585,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -22071,7 +22071,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -22086,7 +22086,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -22124,7 +22124,7 @@
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -22139,7 +22139,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -22214,8 +22214,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
+      <c r="B23" s="232"/>
+      <c r="C23" s="232"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>

</xml_diff>

<commit_message>
change 15 to 30 in data definitions for mrss
</commit_message>
<xml_diff>
--- a/data/imports/mrss-export.xlsx
+++ b/data/imports/mrss-export.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24816"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22360" windowHeight="19380"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22360" windowHeight="19380" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="DataEntry" sheetId="1" r:id="rId1"/>
@@ -5161,13 +5161,7 @@
     <t>Number of Academic Year 2013 Student Credit Hours</t>
   </si>
   <si>
-    <t>FTE Faculty will equal instructor credit hours taught by all full-time credit faculty in the 2013 academic year divided by 15. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
-  </si>
-  <si>
     <t>Enter the number of student credit hours taught by full-time faculty in the 2013 academic year. This should be the number of credit hours for a course times the number of students enrolled in the course (include students who received a grade of W). For example, a 3 credit hour course with 30 enrolled students would generate 90 student credit hours. Exclude high school students taking classes taught by high school faculty in their high schools for college credit. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
-  </si>
-  <si>
-    <t>FTE part-time credit faculty will equal instructor credit hours taught by all part-time faculty or adjuncts in the 2013 academic year divided by 15. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
   </si>
   <si>
     <t>Enter the number of student credit hours taught by part-time faculty or adjuncts in the 2013 academic year. This should be the number of credit hours for a course times the number of students enrolled in the course (include students who received a grade of W). For example, a 3 credit hour course with 30 enrolled students would generate 90 student credit hours. Exclude high school students taking classes taught by high school faculty in their high schools for college credit. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
@@ -5247,12 +5241,6 @@
     <t>Enter the number of student credit hours taught by full-time faculty in the academic unit in the 2013 academic year. This should be the number of credit hours for a course times the number of students enrolled in the course (include students who received a grade of W). For example, a 3 credit hour course with 30 enrolled students would generate 90 student credit hours. Exclude high school students taking classes taught by high school faculty in their high schools for college credit. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
   </si>
   <si>
-    <t>Full-time equivalent (FTE) faculty will equal instructor credit hours taught by all full-time credit faculty in the academic unit in the 2013 academic year divided by 15. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
-  </si>
-  <si>
-    <t>Full-time equivalent (FTE) faculty will equal instructor credit hours taught by all part-time credit faculty or adjuncts in the academic unit in the 2013 academic year divided by 15. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
-  </si>
-  <si>
     <t>Enter the number of student credit hours taught by part-time faculty or adjuncts in the academic unit in the 2013 academic year. This should be the number of credit hours for a course times the number of students enrolled in the course (include students who received a grade of W). For example, a 3 credit hour course with 30 enrolled students would generate 90 student credit hours. Exclude high school students taking classes taught by high school faculty in their high schools for college credit. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
   </si>
   <si>
@@ -5263,6 +5251,18 @@
   </si>
   <si>
     <t>2013 Annual Number of FTE Staff</t>
+  </si>
+  <si>
+    <t>Full-time equivalent (FTE) faculty will equal instructor credit hours taught by all part-time credit faculty or adjuncts in the academic unit in the 2013 academic year divided by 30. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
+  </si>
+  <si>
+    <t>Full-time equivalent (FTE) faculty will equal instructor credit hours taught by all full-time credit faculty in the academic unit in the 2013 academic year divided by 30. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
+  </si>
+  <si>
+    <t>FTE Faculty will equal instructor credit hours taught by all full-time credit faculty in the 2013 academic year divided by 30. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
+  </si>
+  <si>
+    <t>FTE part-time credit faculty will equal instructor credit hours taught by all part-time faculty or adjuncts in the 2013 academic year divided by 30. The 2013 academic year is the end of term counts for summer 2012, fall 2012 and spring 2013.</t>
   </si>
 </sst>
 </file>
@@ -6362,28 +6362,26 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="33" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
@@ -6399,16 +6397,18 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="15"/>
     </xf>
@@ -7342,8 +7342,8 @@
   </sheetPr>
   <dimension ref="A1:X509"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView showGridLines="0" topLeftCell="A237" workbookViewId="0">
+      <selection activeCell="B253" sqref="B253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7359,11 +7359,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="9" customFormat="1" ht="66.5" customHeight="1">
-      <c r="A1" s="230" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="230"/>
-      <c r="C1" s="230"/>
+      <c r="A1" s="243" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
       <c r="D1" s="42"/>
       <c r="E1" s="42"/>
       <c r="F1" s="10"/>
@@ -7396,21 +7396,21 @@
       <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:24" s="11" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A4" s="234" t="s">
+      <c r="A4" s="245" t="s">
         <v>521</v>
       </c>
-      <c r="B4" s="235"/>
-      <c r="C4" s="235"/>
+      <c r="B4" s="246"/>
+      <c r="C4" s="246"/>
       <c r="D4" s="190"/>
       <c r="E4" s="190"/>
       <c r="F4" s="10"/>
     </row>
     <row r="6" spans="1:24" ht="48.75" customHeight="1">
-      <c r="A6" s="233" t="s">
+      <c r="A6" s="244" t="s">
         <v>522</v>
       </c>
-      <c r="B6" s="233"/>
-      <c r="C6" s="233"/>
+      <c r="B6" s="244"/>
+      <c r="C6" s="244"/>
       <c r="D6" s="191"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
@@ -7441,11 +7441,11 @@
       <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:24" s="171" customFormat="1" ht="40" customHeight="1">
-      <c r="A8" s="236" t="s">
+      <c r="A8" s="234" t="s">
         <v>685</v>
       </c>
-      <c r="B8" s="237"/>
-      <c r="C8" s="237"/>
+      <c r="B8" s="235"/>
+      <c r="C8" s="235"/>
       <c r="D8" s="42"/>
       <c r="E8" s="42"/>
       <c r="F8" s="18"/>
@@ -7470,7 +7470,7 @@
     </row>
     <row r="9" spans="1:24" s="64" customFormat="1" ht="24" customHeight="1">
       <c r="A9" s="176" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="B9" s="71"/>
       <c r="C9" s="70"/>
@@ -7553,11 +7553,11 @@
       <c r="X11" s="69"/>
     </row>
     <row r="12" spans="1:24" s="64" customFormat="1" ht="18" customHeight="1">
-      <c r="A12" s="231" t="s">
+      <c r="A12" s="232" t="s">
         <v>456</v>
       </c>
-      <c r="B12" s="232"/>
-      <c r="C12" s="232"/>
+      <c r="B12" s="233"/>
+      <c r="C12" s="233"/>
       <c r="D12" s="192"/>
       <c r="E12" s="192"/>
       <c r="F12" s="69"/>
@@ -7645,7 +7645,7 @@
     </row>
     <row r="16" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A16" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B16" s="80"/>
       <c r="C16" s="48" t="s">
@@ -7660,11 +7660,11 @@
     </row>
     <row r="17" spans="1:24" ht="39" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B17" s="81"/>
       <c r="C17" s="48" t="s">
-        <v>983</v>
+        <v>1003</v>
       </c>
       <c r="D17" s="192" t="s">
         <v>533</v>
@@ -7679,7 +7679,7 @@
       </c>
       <c r="B18" s="81"/>
       <c r="C18" s="48" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="D18" s="192" t="s">
         <v>534</v>
@@ -7698,7 +7698,7 @@
     </row>
     <row r="20" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A20" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B20" s="80"/>
       <c r="C20" s="49" t="s">
@@ -7713,11 +7713,11 @@
     </row>
     <row r="21" spans="1:24" ht="52.5" customHeight="1" thickBot="1">
       <c r="A21" s="229" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="B21" s="81"/>
       <c r="C21" s="49" t="s">
-        <v>985</v>
+        <v>1004</v>
       </c>
       <c r="D21" s="34" t="s">
         <v>536</v>
@@ -7732,7 +7732,7 @@
       </c>
       <c r="B22" s="81"/>
       <c r="C22" s="49" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="D22" s="42" t="s">
         <v>537</v>
@@ -7771,7 +7771,7 @@
     </row>
     <row r="24" spans="1:24" ht="49" thickBot="1">
       <c r="A24" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B24" s="80"/>
       <c r="C24" s="227" t="s">
@@ -7786,11 +7786,11 @@
     </row>
     <row r="25" spans="1:24" ht="47.25" customHeight="1" thickBot="1">
       <c r="A25" s="75" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
       <c r="B25" s="81"/>
       <c r="C25" s="65" t="s">
-        <v>1002</v>
+        <v>998</v>
       </c>
       <c r="D25" s="42" t="s">
         <v>724</v>
@@ -7829,7 +7829,7 @@
     </row>
     <row r="27" spans="1:24" ht="48" customHeight="1" thickBot="1">
       <c r="A27" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B27" s="80"/>
       <c r="C27" s="49" t="s">
@@ -7844,11 +7844,11 @@
     </row>
     <row r="28" spans="1:24" ht="46.5" customHeight="1" thickBot="1">
       <c r="A28" s="75" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
       <c r="B28" s="81"/>
       <c r="C28" s="49" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
       <c r="D28" s="42" t="s">
         <v>539</v>
@@ -7859,7 +7859,7 @@
     </row>
     <row r="29" spans="1:24" ht="49.5" customHeight="1" thickBot="1">
       <c r="A29" s="78" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="B29" s="80"/>
       <c r="C29" s="48" t="s">
@@ -7881,11 +7881,11 @@
       <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:24" ht="40" customHeight="1">
-      <c r="A31" s="236" t="s">
+      <c r="A31" s="234" t="s">
         <v>457</v>
       </c>
-      <c r="B31" s="237"/>
-      <c r="C31" s="237"/>
+      <c r="B31" s="235"/>
+      <c r="C31" s="235"/>
       <c r="F31" s="18"/>
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
@@ -7908,7 +7908,7 @@
     </row>
     <row r="32" spans="1:24" s="64" customFormat="1" ht="24" customHeight="1">
       <c r="A32" s="176" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B32" s="71"/>
       <c r="C32" s="70"/>
@@ -8217,10 +8217,10 @@
       <c r="F49" s="10"/>
     </row>
     <row r="50" spans="1:24" ht="40" customHeight="1">
-      <c r="A50" s="236" t="s">
+      <c r="A50" s="234" t="s">
         <v>470</v>
       </c>
-      <c r="B50" s="237"/>
+      <c r="B50" s="235"/>
       <c r="C50" s="59"/>
       <c r="F50" s="18"/>
       <c r="G50" s="18"/>
@@ -8327,11 +8327,11 @@
       <c r="X53" s="69"/>
     </row>
     <row r="54" spans="1:24" s="64" customFormat="1" ht="18" customHeight="1">
-      <c r="A54" s="231" t="s">
+      <c r="A54" s="232" t="s">
         <v>456</v>
       </c>
-      <c r="B54" s="232"/>
-      <c r="C54" s="232"/>
+      <c r="B54" s="233"/>
+      <c r="C54" s="233"/>
       <c r="D54" s="42"/>
       <c r="E54" s="192"/>
       <c r="F54" s="69"/>
@@ -8384,8 +8384,8 @@
       <c r="A56" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="243"/>
-      <c r="C56" s="244"/>
+      <c r="B56" s="236"/>
+      <c r="C56" s="237"/>
       <c r="F56" s="32"/>
       <c r="G56" s="32"/>
       <c r="H56" s="32"/>
@@ -9354,10 +9354,10 @@
       <c r="F124" s="10"/>
     </row>
     <row r="125" spans="1:24" s="171" customFormat="1" ht="40" customHeight="1">
-      <c r="A125" s="236" t="s">
+      <c r="A125" s="234" t="s">
         <v>689</v>
       </c>
-      <c r="B125" s="237"/>
+      <c r="B125" s="235"/>
       <c r="C125" s="59"/>
       <c r="D125" s="42"/>
       <c r="E125" s="42"/>
@@ -9438,11 +9438,11 @@
       <c r="X127" s="69"/>
     </row>
     <row r="128" spans="1:24" s="64" customFormat="1" ht="18" customHeight="1">
-      <c r="A128" s="231" t="s">
+      <c r="A128" s="232" t="s">
         <v>456</v>
       </c>
-      <c r="B128" s="232"/>
-      <c r="C128" s="232"/>
+      <c r="B128" s="233"/>
+      <c r="C128" s="233"/>
       <c r="D128" s="33"/>
       <c r="E128" s="192"/>
       <c r="F128" s="69"/>
@@ -9495,8 +9495,8 @@
       <c r="A130" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="B130" s="243"/>
-      <c r="C130" s="244"/>
+      <c r="B130" s="236"/>
+      <c r="C130" s="237"/>
       <c r="D130" s="33"/>
       <c r="F130" s="14"/>
       <c r="G130" s="14"/>
@@ -9581,8 +9581,8 @@
       <c r="A136" s="103" t="s">
         <v>71</v>
       </c>
-      <c r="B136" s="243"/>
-      <c r="C136" s="244"/>
+      <c r="B136" s="236"/>
+      <c r="C136" s="237"/>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
       <c r="H136" s="14"/>
@@ -9748,10 +9748,10 @@
       <c r="F147" s="10"/>
     </row>
     <row r="148" spans="1:24" s="61" customFormat="1" ht="40" customHeight="1">
-      <c r="A148" s="236" t="s">
+      <c r="A148" s="234" t="s">
         <v>476</v>
       </c>
-      <c r="B148" s="237"/>
+      <c r="B148" s="235"/>
       <c r="C148" s="59"/>
       <c r="D148" s="42"/>
       <c r="E148" s="42"/>
@@ -9804,11 +9804,11 @@
       <c r="X149" s="69"/>
     </row>
     <row r="150" spans="1:24" s="64" customFormat="1" ht="24" customHeight="1">
-      <c r="A150" s="231" t="s">
+      <c r="A150" s="232" t="s">
         <v>478</v>
       </c>
-      <c r="B150" s="232"/>
-      <c r="C150" s="232"/>
+      <c r="B150" s="233"/>
+      <c r="C150" s="233"/>
       <c r="D150" s="42"/>
       <c r="E150" s="192"/>
       <c r="F150" s="69"/>
@@ -9858,10 +9858,10 @@
       <c r="X151" s="97"/>
     </row>
     <row r="152" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A152" s="245" t="s">
+      <c r="A152" s="230" t="s">
         <v>479</v>
       </c>
-      <c r="B152" s="246"/>
+      <c r="B152" s="231"/>
       <c r="C152" s="107"/>
       <c r="D152" s="42"/>
       <c r="E152" s="42"/>
@@ -9945,10 +9945,10 @@
       <c r="H156" s="14"/>
     </row>
     <row r="157" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A157" s="245" t="s">
+      <c r="A157" s="230" t="s">
         <v>480</v>
       </c>
-      <c r="B157" s="246"/>
+      <c r="B157" s="231"/>
       <c r="C157" s="107"/>
       <c r="D157" s="42" t="s">
         <v>740</v>
@@ -10201,10 +10201,10 @@
       <c r="H172" s="14"/>
     </row>
     <row r="173" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A173" s="245" t="s">
+      <c r="A173" s="230" t="s">
         <v>481</v>
       </c>
-      <c r="B173" s="246"/>
+      <c r="B173" s="231"/>
       <c r="C173" s="107"/>
       <c r="D173" s="42"/>
       <c r="E173" s="42"/>
@@ -10361,10 +10361,10 @@
       <c r="H183" s="14"/>
     </row>
     <row r="184" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A184" s="245" t="s">
+      <c r="A184" s="230" t="s">
         <v>491</v>
       </c>
-      <c r="B184" s="246"/>
+      <c r="B184" s="231"/>
       <c r="C184" s="107"/>
       <c r="D184" s="42"/>
       <c r="E184" s="42"/>
@@ -10431,10 +10431,10 @@
       <c r="H187" s="14"/>
     </row>
     <row r="188" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A188" s="245" t="s">
+      <c r="A188" s="230" t="s">
         <v>492</v>
       </c>
-      <c r="B188" s="246"/>
+      <c r="B188" s="231"/>
       <c r="C188" s="107"/>
       <c r="D188" s="42"/>
       <c r="E188" s="42"/>
@@ -10534,10 +10534,10 @@
       <c r="H194" s="14"/>
     </row>
     <row r="195" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A195" s="245" t="s">
+      <c r="A195" s="230" t="s">
         <v>115</v>
       </c>
-      <c r="B195" s="246"/>
+      <c r="B195" s="231"/>
       <c r="C195" s="107"/>
       <c r="D195" s="42"/>
       <c r="E195" s="42"/>
@@ -10675,10 +10675,10 @@
       <c r="H202" s="42"/>
     </row>
     <row r="203" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A203" s="245" t="s">
+      <c r="A203" s="230" t="s">
         <v>502</v>
       </c>
-      <c r="B203" s="246"/>
+      <c r="B203" s="231"/>
       <c r="C203" s="107"/>
       <c r="D203" s="42"/>
       <c r="E203" s="42"/>
@@ -10779,10 +10779,10 @@
       <c r="F208" s="10"/>
     </row>
     <row r="209" spans="1:24" s="61" customFormat="1" ht="40" customHeight="1">
-      <c r="A209" s="236" t="s">
+      <c r="A209" s="234" t="s">
         <v>503</v>
       </c>
-      <c r="B209" s="237"/>
+      <c r="B209" s="235"/>
       <c r="C209" s="59"/>
       <c r="D209" s="42"/>
       <c r="E209" s="42"/>
@@ -10868,8 +10868,8 @@
       <c r="A212" s="238" t="s">
         <v>706</v>
       </c>
-      <c r="B212" s="232"/>
-      <c r="C212" s="232"/>
+      <c r="B212" s="233"/>
+      <c r="C212" s="233"/>
       <c r="D212" s="42"/>
       <c r="E212" s="192"/>
       <c r="F212" s="69"/>
@@ -10893,10 +10893,10 @@
       <c r="X212" s="69"/>
     </row>
     <row r="213" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A213" s="245" t="s">
+      <c r="A213" s="230" t="s">
         <v>504</v>
       </c>
-      <c r="B213" s="246"/>
+      <c r="B213" s="231"/>
       <c r="C213" s="107"/>
       <c r="D213" s="42"/>
       <c r="E213" s="42"/>
@@ -10982,10 +10982,10 @@
       <c r="H217" s="14"/>
     </row>
     <row r="218" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A218" s="245" t="s">
+      <c r="A218" s="230" t="s">
         <v>504</v>
       </c>
-      <c r="B218" s="246"/>
+      <c r="B218" s="231"/>
       <c r="C218" s="107"/>
       <c r="D218" s="42"/>
       <c r="E218" s="42"/>
@@ -11070,10 +11070,10 @@
       <c r="H222" s="14"/>
     </row>
     <row r="223" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A223" s="245" t="s">
+      <c r="A223" s="230" t="s">
         <v>504</v>
       </c>
-      <c r="B223" s="246"/>
+      <c r="B223" s="231"/>
       <c r="C223" s="107"/>
       <c r="D223" s="42"/>
       <c r="E223" s="42"/>
@@ -11153,10 +11153,10 @@
       <c r="H227" s="14"/>
     </row>
     <row r="228" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A228" s="245" t="s">
+      <c r="A228" s="230" t="s">
         <v>504</v>
       </c>
-      <c r="B228" s="246"/>
+      <c r="B228" s="231"/>
       <c r="C228" s="107"/>
       <c r="D228" s="42"/>
       <c r="E228" s="42"/>
@@ -15766,6 +15766,21 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="31">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A212:C212"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A125:B125"/>
     <mergeCell ref="A213:B213"/>
     <mergeCell ref="A218:B218"/>
     <mergeCell ref="A228:B228"/>
@@ -15782,21 +15797,6 @@
     <mergeCell ref="A188:B188"/>
     <mergeCell ref="A195:B195"/>
     <mergeCell ref="A203:B203"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A212:C212"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A8:C8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A36" location="'Move or Copy'!A1" display="Link to Move or Copy"/>
@@ -15837,7 +15837,7 @@
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -15947,7 +15947,7 @@
     </row>
     <row r="7" spans="1:25" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -16050,12 +16050,12 @@
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -16065,12 +16065,12 @@
     </row>
     <row r="14" spans="1:25" ht="48" customHeight="1" thickBot="1">
       <c r="A14" s="75" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -16085,7 +16085,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -16103,12 +16103,12 @@
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -16118,12 +16118,12 @@
     </row>
     <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -16138,7 +16138,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -16213,8 +16213,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -16465,8 +16465,8 @@
   </sheetPr>
   <dimension ref="A1:Y37"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -16576,7 +16576,7 @@
     </row>
     <row r="7" spans="1:25" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -16632,7 +16632,7 @@
     </row>
     <row r="9" spans="1:25" s="130" customFormat="1" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="131" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="B9" s="127"/>
       <c r="C9" s="127"/>
@@ -16679,12 +16679,12 @@
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -16699,7 +16699,7 @@
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -16714,7 +16714,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -16732,12 +16732,12 @@
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -16752,7 +16752,7 @@
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -16767,7 +16767,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -16842,8 +16842,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -17119,8 +17119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y496"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -17207,7 +17207,7 @@
       <c r="W5" s="3"/>
     </row>
     <row r="6" spans="1:25" s="171" customFormat="1" ht="36" customHeight="1">
-      <c r="A6" s="236" t="s">
+      <c r="A6" s="234" t="s">
         <v>701</v>
       </c>
       <c r="B6" s="254"/>
@@ -17236,7 +17236,7 @@
     </row>
     <row r="7" spans="1:25" s="62" customFormat="1" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -17341,12 +17341,12 @@
     </row>
     <row r="13" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="14"/>
@@ -17356,12 +17356,12 @@
     </row>
     <row r="14" spans="1:25" s="1" customFormat="1" ht="48" customHeight="1" thickBot="1">
       <c r="A14" s="75" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="180" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="14"/>
@@ -17376,7 +17376,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="180" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="13"/>
@@ -17398,12 +17398,12 @@
     </row>
     <row r="17" spans="1:24" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="14"/>
@@ -17413,12 +17413,12 @@
     </row>
     <row r="18" spans="1:24" s="1" customFormat="1" ht="55.5" customHeight="1" thickBot="1">
       <c r="A18" s="75" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="135"/>
       <c r="D18" s="180" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="14"/>
@@ -17433,7 +17433,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="66"/>
       <c r="D19" s="140" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
@@ -17507,8 +17507,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -18066,7 +18066,7 @@
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -18176,7 +18176,7 @@
     </row>
     <row r="7" spans="1:25" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -18279,12 +18279,12 @@
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -18294,12 +18294,12 @@
     </row>
     <row r="14" spans="1:25" ht="48" customHeight="1" thickBot="1">
       <c r="A14" s="76" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="180" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -18314,7 +18314,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="180" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -18332,12 +18332,12 @@
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -18347,12 +18347,12 @@
     </row>
     <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="180" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -18367,7 +18367,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -18442,8 +18442,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -18692,7 +18692,7 @@
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -18802,7 +18802,7 @@
     </row>
     <row r="7" spans="1:25" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -18905,12 +18905,12 @@
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -18920,12 +18920,12 @@
     </row>
     <row r="14" spans="1:25" ht="48" customHeight="1" thickBot="1">
       <c r="A14" s="76" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -18940,7 +18940,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -18958,12 +18958,12 @@
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -18973,12 +18973,12 @@
     </row>
     <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -18993,7 +18993,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -19068,8 +19068,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -19318,7 +19318,7 @@
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -19428,7 +19428,7 @@
     </row>
     <row r="7" spans="1:25" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -19531,12 +19531,12 @@
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -19546,12 +19546,12 @@
     </row>
     <row r="14" spans="1:25" ht="48" customHeight="1" thickBot="1">
       <c r="A14" s="76" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -19566,7 +19566,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42" t="s">
@@ -19586,12 +19586,12 @@
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -19601,12 +19601,12 @@
     </row>
     <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -19621,7 +19621,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -19696,8 +19696,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -19949,7 +19949,7 @@
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -20059,7 +20059,7 @@
     </row>
     <row r="7" spans="1:25" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -20164,12 +20164,12 @@
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -20179,12 +20179,12 @@
     </row>
     <row r="14" spans="1:25" ht="48" customHeight="1" thickBot="1">
       <c r="A14" s="76" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -20199,7 +20199,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -20217,12 +20217,12 @@
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -20232,12 +20232,12 @@
     </row>
     <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -20252,7 +20252,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -20327,8 +20327,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -20580,7 +20580,7 @@
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -20690,7 +20690,7 @@
     </row>
     <row r="7" spans="1:25" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -20793,12 +20793,12 @@
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -20808,12 +20808,12 @@
     </row>
     <row r="14" spans="1:25" ht="48" customHeight="1" thickBot="1">
       <c r="A14" s="76" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -20828,7 +20828,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -20846,12 +20846,12 @@
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -20861,12 +20861,12 @@
     </row>
     <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -20881,7 +20881,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -20956,8 +20956,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -21209,7 +21209,7 @@
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -21319,7 +21319,7 @@
     </row>
     <row r="7" spans="1:25" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -21375,7 +21375,7 @@
     </row>
     <row r="9" spans="1:25" s="130" customFormat="1" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="131" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="B9" s="127"/>
       <c r="C9" s="127"/>
@@ -21422,12 +21422,12 @@
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -21437,12 +21437,12 @@
     </row>
     <row r="14" spans="1:25" ht="48" customHeight="1" thickBot="1">
       <c r="A14" s="76" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -21457,7 +21457,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -21475,12 +21475,12 @@
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -21490,12 +21490,12 @@
     </row>
     <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -21510,7 +21510,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -21585,8 +21585,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -21838,7 +21838,7 @@
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -21948,7 +21948,7 @@
     </row>
     <row r="7" spans="1:25" ht="23.25" customHeight="1">
       <c r="A7" s="260" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B7" s="259"/>
       <c r="C7" s="93"/>
@@ -22004,7 +22004,7 @@
     </row>
     <row r="9" spans="1:25" s="130" customFormat="1" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="131" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="B9" s="127"/>
       <c r="C9" s="127"/>
@@ -22051,12 +22051,12 @@
     </row>
     <row r="13" spans="1:25" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B13" s="134"/>
       <c r="C13" s="136"/>
       <c r="D13" s="140" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
@@ -22066,12 +22066,12 @@
     </row>
     <row r="14" spans="1:25" ht="48" customHeight="1" thickBot="1">
       <c r="A14" s="76" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B14" s="134"/>
       <c r="C14" s="226"/>
       <c r="D14" s="140" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -22086,7 +22086,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="81"/>
       <c r="D15" s="140" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -22104,12 +22104,12 @@
     </row>
     <row r="17" spans="1:24" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="75" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="137"/>
       <c r="D17" s="140" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -22119,12 +22119,12 @@
     </row>
     <row r="18" spans="1:24" ht="56" customHeight="1" thickBot="1">
       <c r="A18" s="76" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B18" s="134"/>
       <c r="C18" s="226"/>
       <c r="D18" s="140" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
@@ -22139,7 +22139,7 @@
       <c r="B19" s="134"/>
       <c r="C19" s="81"/>
       <c r="D19" s="140" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
@@ -22214,8 +22214,8 @@
       <c r="A23" s="256" t="s">
         <v>684</v>
       </c>
-      <c r="B23" s="232"/>
-      <c r="C23" s="232"/>
+      <c r="B23" s="233"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>

</xml_diff>

<commit_message>
fix excel for mrss
</commit_message>
<xml_diff>
--- a/data/imports/mrss-export.xlsx
+++ b/data/imports/mrss-export.xlsx
@@ -6361,28 +6361,26 @@
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="33" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
@@ -6398,16 +6396,18 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="15"/>
     </xf>
@@ -7403,11 +7403,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="9" customFormat="1" ht="66.5" customHeight="1">
-      <c r="A1" s="234" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="234"/>
-      <c r="C1" s="234"/>
+      <c r="A1" s="247" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="247"/>
+      <c r="C1" s="247"/>
       <c r="D1" s="42"/>
       <c r="E1" s="42"/>
       <c r="F1" s="10"/>
@@ -7440,21 +7440,21 @@
       <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:24" s="11" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A4" s="238" t="s">
+      <c r="A4" s="249" t="s">
         <v>519</v>
       </c>
-      <c r="B4" s="239"/>
-      <c r="C4" s="239"/>
+      <c r="B4" s="250"/>
+      <c r="C4" s="250"/>
       <c r="D4" s="190"/>
       <c r="E4" s="190"/>
       <c r="F4" s="10"/>
     </row>
     <row r="6" spans="1:24" ht="48.75" customHeight="1">
-      <c r="A6" s="237" t="s">
+      <c r="A6" s="248" t="s">
         <v>520</v>
       </c>
-      <c r="B6" s="237"/>
-      <c r="C6" s="237"/>
+      <c r="B6" s="248"/>
+      <c r="C6" s="248"/>
       <c r="D6" s="191"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
@@ -7485,11 +7485,11 @@
       <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:24" s="171" customFormat="1" ht="40" customHeight="1">
-      <c r="A8" s="240" t="s">
+      <c r="A8" s="238" t="s">
         <v>683</v>
       </c>
-      <c r="B8" s="241"/>
-      <c r="C8" s="241"/>
+      <c r="B8" s="239"/>
+      <c r="C8" s="239"/>
       <c r="D8" s="42"/>
       <c r="E8" s="42"/>
       <c r="F8" s="18"/>
@@ -7597,11 +7597,11 @@
       <c r="X11" s="69"/>
     </row>
     <row r="12" spans="1:24" s="64" customFormat="1" ht="18" customHeight="1">
-      <c r="A12" s="235" t="s">
+      <c r="A12" s="236" t="s">
         <v>455</v>
       </c>
-      <c r="B12" s="236"/>
-      <c r="C12" s="236"/>
+      <c r="B12" s="237"/>
+      <c r="C12" s="237"/>
       <c r="D12" s="192"/>
       <c r="E12" s="192"/>
       <c r="F12" s="69"/>
@@ -7925,11 +7925,11 @@
       <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:24" ht="40" customHeight="1">
-      <c r="A31" s="240" t="s">
+      <c r="A31" s="238" t="s">
         <v>456</v>
       </c>
-      <c r="B31" s="241"/>
-      <c r="C31" s="241"/>
+      <c r="B31" s="239"/>
+      <c r="C31" s="239"/>
       <c r="F31" s="18"/>
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
@@ -8261,10 +8261,10 @@
       <c r="F49" s="10"/>
     </row>
     <row r="50" spans="1:24" ht="40" customHeight="1">
-      <c r="A50" s="240" t="s">
+      <c r="A50" s="238" t="s">
         <v>469</v>
       </c>
-      <c r="B50" s="241"/>
+      <c r="B50" s="239"/>
       <c r="C50" s="59"/>
       <c r="F50" s="18"/>
       <c r="G50" s="18"/>
@@ -8371,11 +8371,11 @@
       <c r="X53" s="69"/>
     </row>
     <row r="54" spans="1:24" s="64" customFormat="1" ht="18" customHeight="1">
-      <c r="A54" s="235" t="s">
+      <c r="A54" s="236" t="s">
         <v>455</v>
       </c>
-      <c r="B54" s="236"/>
-      <c r="C54" s="236"/>
+      <c r="B54" s="237"/>
+      <c r="C54" s="237"/>
       <c r="D54" s="42"/>
       <c r="E54" s="192"/>
       <c r="F54" s="69"/>
@@ -8428,8 +8428,8 @@
       <c r="A56" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="247"/>
-      <c r="C56" s="248"/>
+      <c r="B56" s="240"/>
+      <c r="C56" s="241"/>
       <c r="F56" s="32"/>
       <c r="G56" s="32"/>
       <c r="H56" s="32"/>
@@ -9398,10 +9398,10 @@
       <c r="F124" s="10"/>
     </row>
     <row r="125" spans="1:24" s="171" customFormat="1" ht="40" customHeight="1">
-      <c r="A125" s="240" t="s">
+      <c r="A125" s="238" t="s">
         <v>687</v>
       </c>
-      <c r="B125" s="241"/>
+      <c r="B125" s="239"/>
       <c r="C125" s="59"/>
       <c r="D125" s="42"/>
       <c r="E125" s="42"/>
@@ -9482,11 +9482,11 @@
       <c r="X127" s="69"/>
     </row>
     <row r="128" spans="1:24" s="64" customFormat="1" ht="18" customHeight="1">
-      <c r="A128" s="235" t="s">
+      <c r="A128" s="236" t="s">
         <v>455</v>
       </c>
-      <c r="B128" s="236"/>
-      <c r="C128" s="236"/>
+      <c r="B128" s="237"/>
+      <c r="C128" s="237"/>
       <c r="D128" s="33"/>
       <c r="E128" s="192"/>
       <c r="F128" s="69"/>
@@ -9539,8 +9539,8 @@
       <c r="A130" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="B130" s="247"/>
-      <c r="C130" s="248"/>
+      <c r="B130" s="240"/>
+      <c r="C130" s="241"/>
       <c r="D130" s="33"/>
       <c r="F130" s="14"/>
       <c r="G130" s="14"/>
@@ -9625,8 +9625,8 @@
       <c r="A136" s="103" t="s">
         <v>71</v>
       </c>
-      <c r="B136" s="247"/>
-      <c r="C136" s="248"/>
+      <c r="B136" s="240"/>
+      <c r="C136" s="241"/>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
       <c r="H136" s="14"/>
@@ -9792,10 +9792,10 @@
       <c r="F147" s="10"/>
     </row>
     <row r="148" spans="1:24" s="61" customFormat="1" ht="40" customHeight="1">
-      <c r="A148" s="240" t="s">
+      <c r="A148" s="238" t="s">
         <v>475</v>
       </c>
-      <c r="B148" s="241"/>
+      <c r="B148" s="239"/>
       <c r="C148" s="59"/>
       <c r="D148" s="42"/>
       <c r="E148" s="42"/>
@@ -9848,11 +9848,11 @@
       <c r="X149" s="69"/>
     </row>
     <row r="150" spans="1:24" s="64" customFormat="1" ht="24" customHeight="1">
-      <c r="A150" s="235" t="s">
+      <c r="A150" s="236" t="s">
         <v>477</v>
       </c>
-      <c r="B150" s="236"/>
-      <c r="C150" s="236"/>
+      <c r="B150" s="237"/>
+      <c r="C150" s="237"/>
       <c r="D150" s="42"/>
       <c r="E150" s="192"/>
       <c r="F150" s="69"/>
@@ -9902,10 +9902,10 @@
       <c r="X151" s="97"/>
     </row>
     <row r="152" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A152" s="249" t="s">
+      <c r="A152" s="234" t="s">
         <v>478</v>
       </c>
-      <c r="B152" s="250"/>
+      <c r="B152" s="235"/>
       <c r="C152" s="107"/>
       <c r="D152" s="42"/>
       <c r="E152" s="42"/>
@@ -9989,10 +9989,10 @@
       <c r="H156" s="14"/>
     </row>
     <row r="157" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A157" s="249" t="s">
+      <c r="A157" s="234" t="s">
         <v>479</v>
       </c>
-      <c r="B157" s="250"/>
+      <c r="B157" s="235"/>
       <c r="C157" s="107"/>
       <c r="D157" s="42" t="s">
         <v>738</v>
@@ -10245,10 +10245,10 @@
       <c r="H172" s="14"/>
     </row>
     <row r="173" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A173" s="249" t="s">
+      <c r="A173" s="234" t="s">
         <v>480</v>
       </c>
-      <c r="B173" s="250"/>
+      <c r="B173" s="235"/>
       <c r="C173" s="107"/>
       <c r="D173" s="42"/>
       <c r="E173" s="42"/>
@@ -10405,10 +10405,10 @@
       <c r="H183" s="14"/>
     </row>
     <row r="184" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A184" s="249" t="s">
+      <c r="A184" s="234" t="s">
         <v>490</v>
       </c>
-      <c r="B184" s="250"/>
+      <c r="B184" s="235"/>
       <c r="C184" s="107"/>
       <c r="D184" s="42"/>
       <c r="E184" s="42"/>
@@ -10475,10 +10475,10 @@
       <c r="H187" s="14"/>
     </row>
     <row r="188" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A188" s="249" t="s">
+      <c r="A188" s="234" t="s">
         <v>491</v>
       </c>
-      <c r="B188" s="250"/>
+      <c r="B188" s="235"/>
       <c r="C188" s="107"/>
       <c r="D188" s="42"/>
       <c r="E188" s="42"/>
@@ -10578,10 +10578,10 @@
       <c r="H194" s="14"/>
     </row>
     <row r="195" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A195" s="249" t="s">
+      <c r="A195" s="234" t="s">
         <v>115</v>
       </c>
-      <c r="B195" s="250"/>
+      <c r="B195" s="235"/>
       <c r="C195" s="107"/>
       <c r="D195" s="42"/>
       <c r="E195" s="42"/>
@@ -10719,10 +10719,10 @@
       <c r="H202" s="42"/>
     </row>
     <row r="203" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A203" s="249" t="s">
+      <c r="A203" s="234" t="s">
         <v>501</v>
       </c>
-      <c r="B203" s="250"/>
+      <c r="B203" s="235"/>
       <c r="C203" s="107"/>
       <c r="D203" s="42"/>
       <c r="E203" s="42"/>
@@ -10823,10 +10823,10 @@
       <c r="F208" s="10"/>
     </row>
     <row r="209" spans="1:24" s="61" customFormat="1" ht="40" customHeight="1">
-      <c r="A209" s="240" t="s">
+      <c r="A209" s="238" t="s">
         <v>502</v>
       </c>
-      <c r="B209" s="241"/>
+      <c r="B209" s="239"/>
       <c r="C209" s="59"/>
       <c r="D209" s="42"/>
       <c r="E209" s="42"/>
@@ -10912,8 +10912,8 @@
       <c r="A212" s="242" t="s">
         <v>704</v>
       </c>
-      <c r="B212" s="236"/>
-      <c r="C212" s="236"/>
+      <c r="B212" s="237"/>
+      <c r="C212" s="237"/>
       <c r="D212" s="42"/>
       <c r="E212" s="192"/>
       <c r="F212" s="69"/>
@@ -10937,10 +10937,10 @@
       <c r="X212" s="69"/>
     </row>
     <row r="213" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A213" s="249" t="s">
+      <c r="A213" s="234" t="s">
         <v>503</v>
       </c>
-      <c r="B213" s="250"/>
+      <c r="B213" s="235"/>
       <c r="C213" s="107"/>
       <c r="D213" s="42"/>
       <c r="E213" s="42"/>
@@ -11026,10 +11026,10 @@
       <c r="H217" s="14"/>
     </row>
     <row r="218" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A218" s="249" t="s">
+      <c r="A218" s="234" t="s">
         <v>503</v>
       </c>
-      <c r="B218" s="250"/>
+      <c r="B218" s="235"/>
       <c r="C218" s="107"/>
       <c r="D218" s="42"/>
       <c r="E218" s="42"/>
@@ -11114,10 +11114,10 @@
       <c r="H222" s="14"/>
     </row>
     <row r="223" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A223" s="249" t="s">
+      <c r="A223" s="234" t="s">
         <v>503</v>
       </c>
-      <c r="B223" s="250"/>
+      <c r="B223" s="235"/>
       <c r="C223" s="107"/>
       <c r="D223" s="42"/>
       <c r="E223" s="42"/>
@@ -11197,10 +11197,10 @@
       <c r="H227" s="14"/>
     </row>
     <row r="228" spans="1:24" s="61" customFormat="1" ht="36" customHeight="1">
-      <c r="A228" s="249" t="s">
+      <c r="A228" s="234" t="s">
         <v>503</v>
       </c>
-      <c r="B228" s="250"/>
+      <c r="B228" s="235"/>
       <c r="C228" s="107"/>
       <c r="D228" s="42"/>
       <c r="E228" s="42"/>
@@ -15810,6 +15810,21 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="31">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A212:C212"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A125:B125"/>
     <mergeCell ref="A213:B213"/>
     <mergeCell ref="A218:B218"/>
     <mergeCell ref="A228:B228"/>
@@ -15826,21 +15841,6 @@
     <mergeCell ref="A188:B188"/>
     <mergeCell ref="A195:B195"/>
     <mergeCell ref="A203:B203"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A212:C212"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A8:C8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A36" location="'Move or Copy'!A1" display="Link to Move or Copy"/>
@@ -15881,7 +15881,7 @@
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -16257,8 +16257,8 @@
       <c r="A23" s="260" t="s">
         <v>682</v>
       </c>
-      <c r="B23" s="236"/>
-      <c r="C23" s="236"/>
+      <c r="B23" s="237"/>
+      <c r="C23" s="237"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -16510,7 +16510,7 @@
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -16886,8 +16886,8 @@
       <c r="A23" s="260" t="s">
         <v>682</v>
       </c>
-      <c r="B23" s="236"/>
-      <c r="C23" s="236"/>
+      <c r="B23" s="237"/>
+      <c r="C23" s="237"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -17251,7 +17251,7 @@
       <c r="W5" s="3"/>
     </row>
     <row r="6" spans="1:25" s="171" customFormat="1" ht="36" customHeight="1">
-      <c r="A6" s="240" t="s">
+      <c r="A6" s="238" t="s">
         <v>699</v>
       </c>
       <c r="B6" s="258"/>
@@ -17551,8 +17551,8 @@
       <c r="A23" s="260" t="s">
         <v>682</v>
       </c>
-      <c r="B23" s="236"/>
-      <c r="C23" s="236"/>
+      <c r="B23" s="237"/>
+      <c r="C23" s="237"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -18486,8 +18486,8 @@
       <c r="A23" s="260" t="s">
         <v>682</v>
       </c>
-      <c r="B23" s="236"/>
-      <c r="C23" s="236"/>
+      <c r="B23" s="237"/>
+      <c r="C23" s="237"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -19112,8 +19112,8 @@
       <c r="A23" s="260" t="s">
         <v>682</v>
       </c>
-      <c r="B23" s="236"/>
-      <c r="C23" s="236"/>
+      <c r="B23" s="237"/>
+      <c r="C23" s="237"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -19740,8 +19740,8 @@
       <c r="A23" s="260" t="s">
         <v>682</v>
       </c>
-      <c r="B23" s="236"/>
-      <c r="C23" s="236"/>
+      <c r="B23" s="237"/>
+      <c r="C23" s="237"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -20371,8 +20371,8 @@
       <c r="A23" s="260" t="s">
         <v>682</v>
       </c>
-      <c r="B23" s="236"/>
-      <c r="C23" s="236"/>
+      <c r="B23" s="237"/>
+      <c r="C23" s="237"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -21000,8 +21000,8 @@
       <c r="A23" s="260" t="s">
         <v>682</v>
       </c>
-      <c r="B23" s="236"/>
-      <c r="C23" s="236"/>
+      <c r="B23" s="237"/>
+      <c r="C23" s="237"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -21629,8 +21629,8 @@
       <c r="A23" s="260" t="s">
         <v>682</v>
       </c>
-      <c r="B23" s="236"/>
-      <c r="C23" s="236"/>
+      <c r="B23" s="237"/>
+      <c r="C23" s="237"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -21881,7 +21881,7 @@
   </sheetPr>
   <dimension ref="A1:Y37"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -22258,8 +22258,8 @@
       <c r="A23" s="260" t="s">
         <v>682</v>
       </c>
-      <c r="B23" s="236"/>
-      <c r="C23" s="236"/>
+      <c r="B23" s="237"/>
+      <c r="C23" s="237"/>
       <c r="D23" s="145"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>

</xml_diff>